<commit_message>
add new run list
</commit_message>
<xml_diff>
--- a/IO_Dev/RunControl_Dev.xlsx
+++ b/IO_Dev/RunControl_Dev.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\PenSim-Projects\Model_Main\IO_Dev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Model_Main\IO_Dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="7230" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="7230" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -1295,11 +1295,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="AC6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AK16" sqref="AK16"/>
+      <selection pane="bottomRight" activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1716,7 +1716,7 @@
         <v>65</v>
       </c>
       <c r="O6">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="P6" s="12">
         <v>0.01</v>
@@ -2098,8 +2098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2137,7 +2137,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <v>1000</v>
@@ -2168,8 +2168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
First version of multiple retirement ages
Not internally consistent
</commit_message>
<xml_diff>
--- a/IO_Dev/RunControl_Dev.xlsx
+++ b/IO_Dev/RunControl_Dev.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Model_Main\IO_Dev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\PenSim-Projects\Model_Main\IO_Dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="7230" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="7230" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -1295,11 +1295,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="O6" sqref="O6"/>
+      <selection pane="bottomRight" activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1704,7 +1704,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6" s="12">
         <v>1.7999999999999999E-2</v>
@@ -1743,7 +1743,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="X6" s="12">
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="Y6" t="s">
         <v>112</v>
@@ -2098,8 +2098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
try to resolve the inconsistency
</commit_message>
<xml_diff>
--- a/IO_Dev/RunControl_Dev.xlsx
+++ b/IO_Dev/RunControl_Dev.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="7230" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="7230" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -509,9 +509,6 @@
     <t>open</t>
   </si>
   <si>
-    <t>cp</t>
-  </si>
-  <si>
     <t>Non-Negative ADC and ERC</t>
   </si>
   <si>
@@ -573,6 +570,9 @@
   </si>
   <si>
     <t>sd</t>
+  </si>
+  <si>
+    <t>cd</t>
   </si>
 </sst>
 </file>
@@ -771,13 +771,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -786,10 +780,16 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1295,11 +1295,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="I28" sqref="I28"/>
+      <selection pane="bottomRight" activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1394,7 +1394,7 @@
         <v>38</v>
       </c>
       <c r="AC2" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AD2" s="6"/>
       <c r="AE2" s="4" t="s">
@@ -1413,10 +1413,10 @@
         <v>40</v>
       </c>
       <c r="AP2" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AQ2" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:43" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1448,7 +1448,7 @@
         <v>51</v>
       </c>
       <c r="AC3" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AD3" s="4"/>
       <c r="AG3" s="4" t="s">
@@ -1471,59 +1471,59 @@
       </c>
     </row>
     <row r="4" spans="1:43" s="8" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="29" t="s">
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="29"/>
-      <c r="F4" s="30" t="s">
+      <c r="E4" s="33"/>
+      <c r="F4" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="30"/>
-      <c r="H4" s="31" t="s">
+      <c r="G4" s="34"/>
+      <c r="H4" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="I4" s="31"/>
-      <c r="J4" s="32" t="s">
+      <c r="I4" s="29"/>
+      <c r="J4" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="K4" s="32"/>
-      <c r="L4" s="31" t="s">
+      <c r="K4" s="30"/>
+      <c r="L4" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="M4" s="31"/>
-      <c r="N4" s="31"/>
-      <c r="O4" s="31"/>
-      <c r="P4" s="31"/>
-      <c r="Q4" s="31"/>
-      <c r="R4" s="31"/>
-      <c r="S4" s="32" t="s">
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="T4" s="32"/>
-      <c r="U4" s="32"/>
-      <c r="V4" s="33" t="s">
+      <c r="T4" s="30"/>
+      <c r="U4" s="30"/>
+      <c r="V4" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="W4" s="33"/>
-      <c r="X4" s="33"/>
+      <c r="W4" s="28"/>
+      <c r="X4" s="28"/>
       <c r="Y4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="Z4" s="28" t="s">
+      <c r="Z4" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="AA4" s="28"/>
-      <c r="AB4" s="28"/>
-      <c r="AC4" s="33" t="s">
+      <c r="AA4" s="31"/>
+      <c r="AB4" s="31"/>
+      <c r="AC4" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="AD4" s="33"/>
-      <c r="AE4" s="33"/>
+      <c r="AD4" s="28"/>
+      <c r="AE4" s="28"/>
       <c r="AF4" s="22" t="s">
         <v>70</v>
       </c>
@@ -1531,12 +1531,12 @@
       <c r="AH4" s="22"/>
       <c r="AI4" s="22"/>
       <c r="AJ4" s="22"/>
-      <c r="AK4" s="34" t="s">
+      <c r="AK4" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="AL4" s="34"/>
-      <c r="AM4" s="34"/>
-      <c r="AN4" s="34"/>
+      <c r="AL4" s="32"/>
+      <c r="AM4" s="32"/>
+      <c r="AN4" s="32"/>
       <c r="AO4" s="16"/>
       <c r="AP4" s="23"/>
       <c r="AQ4" s="21"/>
@@ -1630,7 +1630,7 @@
         <v>106</v>
       </c>
       <c r="AD5" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AE5" s="9" t="s">
         <v>102</v>
@@ -1666,18 +1666,18 @@
         <v>157</v>
       </c>
       <c r="AP5" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AQ5" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C6" s="11" t="b">
         <v>1</v>
@@ -1698,7 +1698,7 @@
         <v>147</v>
       </c>
       <c r="I6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J6" s="12">
         <v>0</v>
@@ -1716,7 +1716,7 @@
         <v>65</v>
       </c>
       <c r="O6">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="P6" s="12">
         <v>0.01</v>
@@ -1752,13 +1752,13 @@
         <v>158</v>
       </c>
       <c r="AA6" s="2" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
       <c r="AB6">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="AC6" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AD6" s="18">
         <v>1</v>
@@ -1767,7 +1767,7 @@
         <v>200</v>
       </c>
       <c r="AF6" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="AG6">
         <v>5</v>
@@ -1826,17 +1826,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
     <mergeCell ref="AC4:AE4"/>
     <mergeCell ref="L4:R4"/>
     <mergeCell ref="S4:U4"/>
     <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="AK4:AN4"/>
     <mergeCell ref="V4:X4"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <dataValidations count="20">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI6">
@@ -2098,8 +2098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2137,7 +2137,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="B3">
         <v>1000</v>
@@ -2299,22 +2299,22 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -2377,7 +2377,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -2395,12 +2395,12 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2427,7 +2427,7 @@
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B2">
         <v>2.7E-2</v>
@@ -2435,7 +2435,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B3">
         <v>0.4</v>
@@ -2443,10 +2443,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B5" t="s">
         <v>179</v>
-      </c>
-      <c r="B5" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
try to resolve inconsistency.
Still no internally consistent.
</commit_message>
<xml_diff>
--- a/IO_Dev/RunControl_Dev.xlsx
+++ b/IO_Dev/RunControl_Dev.xlsx
@@ -1296,10 +1296,10 @@
   <dimension ref="A1:AQ14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="V6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="O11" sqref="O11"/>
+      <selection pane="bottomRight" activeCell="AP10" sqref="AP10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1797,7 +1797,7 @@
         <v>0</v>
       </c>
       <c r="AP6" s="19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ6" s="19" t="b">
         <v>0</v>
@@ -2414,10 +2414,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E13"/>
+  <dimension ref="A2:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B10"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2500,6 +2500,18 @@
         <v>2.6999999999999996E-2</v>
       </c>
     </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f>335869.7 - 310296</f>
+        <v>25573.700000000012</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f xml:space="preserve"> (310296 + 2140.9)*1.075</f>
+        <v>335869.66750000004</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
The first internally consistent version for multiple retirement ages.
Still need to deal with compatibility with  terminations.
</commit_message>
<xml_diff>
--- a/IO_Dev/RunControl_Dev.xlsx
+++ b/IO_Dev/RunControl_Dev.xlsx
@@ -1296,10 +1296,10 @@
   <dimension ref="A1:AQ14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="V6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AP10" sqref="AP10"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1704,10 +1704,10 @@
         <v>0</v>
       </c>
       <c r="K6" s="19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L6" s="12">
-        <v>1.7999999999999999E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="M6">
         <v>3</v>
@@ -1716,10 +1716,10 @@
         <v>65</v>
       </c>
       <c r="O6">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="P6" s="12">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="Q6">
         <v>10</v>
@@ -2099,7 +2099,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2414,10 +2414,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E17"/>
+  <dimension ref="A2:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2512,6 +2512,12 @@
         <v>335869.66750000004</v>
       </c>
     </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="26">
+        <f>(355318.4 - 30244)*1.075</f>
+        <v>349454.98000000004</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
new runs for verifying MRA
</commit_message>
<xml_diff>
--- a/IO_Dev/RunControl_Dev.xlsx
+++ b/IO_Dev/RunControl_Dev.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="190">
   <si>
     <t>Sheet #</t>
   </si>
@@ -542,6 +542,9 @@
     <t>pa-psers</t>
   </si>
   <si>
+    <t>DF100-1</t>
+  </si>
+  <si>
     <t>youngplan</t>
   </si>
   <si>
@@ -572,16 +575,31 @@
     <t>cd</t>
   </si>
   <si>
-    <t>r.full</t>
-  </si>
-  <si>
-    <t>full retirement age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age at which all qualified active members and vested terms start receiving retirement benefits. </t>
-  </si>
-  <si>
-    <t>Dev1</t>
+    <t>O1</t>
+  </si>
+  <si>
+    <t>O2</t>
+  </si>
+  <si>
+    <t>O3</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>M3</t>
   </si>
 </sst>
 </file>
@@ -1302,13 +1320,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR14"/>
+  <dimension ref="A1:AQ19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="H6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="K5" sqref="K5"/>
+      <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1322,32 +1340,32 @@
     <col min="8" max="8" width="24.42578125"/>
     <col min="9" max="9" width="13.42578125" customWidth="1"/>
     <col min="10" max="11" width="13.140625" customWidth="1"/>
-    <col min="12" max="16" width="9.28515625" customWidth="1"/>
-    <col min="17" max="17" width="16"/>
-    <col min="18" max="22" width="12.7109375"/>
-    <col min="23" max="23" width="11.140625" customWidth="1"/>
-    <col min="24" max="28" width="12.7109375"/>
-    <col min="29" max="29" width="12.7109375" customWidth="1"/>
-    <col min="30" max="31" width="11.7109375" customWidth="1"/>
-    <col min="32" max="32" width="13.140625" customWidth="1"/>
-    <col min="33" max="33" width="11.85546875" customWidth="1"/>
-    <col min="38" max="41" width="12.7109375"/>
-    <col min="44" max="44" width="9" customWidth="1"/>
-    <col min="45" max="1031" width="8.5703125"/>
+    <col min="12" max="15" width="9.28515625" customWidth="1"/>
+    <col min="16" max="16" width="16"/>
+    <col min="17" max="21" width="12.7109375"/>
+    <col min="22" max="22" width="11.140625" customWidth="1"/>
+    <col min="23" max="27" width="12.7109375"/>
+    <col min="28" max="28" width="12.7109375" customWidth="1"/>
+    <col min="29" max="30" width="11.7109375" customWidth="1"/>
+    <col min="31" max="31" width="13.140625" customWidth="1"/>
+    <col min="32" max="32" width="11.85546875" customWidth="1"/>
+    <col min="37" max="40" width="12.7109375"/>
+    <col min="43" max="43" width="9" customWidth="1"/>
+    <col min="44" max="1030" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="AL1" s="1" t="s">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AK1" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="AL1" s="1"/>
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="1"/>
-    </row>
-    <row r="2" spans="1:44" s="4" customFormat="1" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:43" s="4" customFormat="1" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
@@ -1382,56 +1400,53 @@
         <v>31</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>181</v>
+        <v>32</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="V2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AB2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AD2" s="6" t="s">
+      <c r="AC2" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="AE2" s="6"/>
-      <c r="AF2" s="4" t="s">
+      <c r="AD2" s="6"/>
+      <c r="AE2" s="4" t="s">
         <v>41</v>
       </c>
+      <c r="AF2" s="6"/>
       <c r="AG2" s="6"/>
-      <c r="AH2" s="6"/>
-      <c r="AJ2" s="6"/>
-      <c r="AK2" s="4" t="s">
+      <c r="AI2" s="6"/>
+      <c r="AJ2" s="4" t="s">
         <v>42</v>
       </c>
+      <c r="AL2" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="AM2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="AN2" s="4" t="s">
         <v>40</v>
       </c>
+      <c r="AP2" s="4" t="s">
+        <v>159</v>
+      </c>
       <c r="AQ2" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="AR2" s="4" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:44" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>43</v>
       </c>
@@ -1456,36 +1471,33 @@
       <c r="O3" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="P3" s="4" t="s">
-        <v>182</v>
+      <c r="AB3" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="AC3" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AD3" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="AE3" s="4"/>
+      <c r="AD3" s="4"/>
+      <c r="AG3" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="AH3" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AI3" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ3" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="AK3" s="4" t="s">
         <v>57</v>
       </c>
+      <c r="AL3" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="AM3" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="AN3" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:44" s="8" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43" s="8" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
         <v>58</v>
       </c>
@@ -1516,48 +1528,47 @@
       <c r="P4" s="31"/>
       <c r="Q4" s="31"/>
       <c r="R4" s="31"/>
-      <c r="S4" s="31"/>
-      <c r="T4" s="32" t="s">
+      <c r="S4" s="32" t="s">
         <v>64</v>
       </c>
+      <c r="T4" s="32"/>
       <c r="U4" s="32"/>
-      <c r="V4" s="32"/>
-      <c r="W4" s="33" t="s">
+      <c r="V4" s="33" t="s">
         <v>65</v>
       </c>
+      <c r="W4" s="33"/>
       <c r="X4" s="33"/>
-      <c r="Y4" s="33"/>
-      <c r="Z4" s="7" t="s">
+      <c r="Y4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AA4" s="28" t="s">
+      <c r="Z4" s="28" t="s">
         <v>67</v>
       </c>
+      <c r="AA4" s="28"/>
       <c r="AB4" s="28"/>
-      <c r="AC4" s="28"/>
-      <c r="AD4" s="33" t="s">
+      <c r="AC4" s="33" t="s">
         <v>69</v>
       </c>
+      <c r="AD4" s="33"/>
       <c r="AE4" s="33"/>
-      <c r="AF4" s="33"/>
-      <c r="AG4" s="22" t="s">
+      <c r="AF4" s="22" t="s">
         <v>70</v>
       </c>
+      <c r="AG4" s="22"/>
       <c r="AH4" s="22"/>
       <c r="AI4" s="22"/>
       <c r="AJ4" s="22"/>
-      <c r="AK4" s="22"/>
-      <c r="AL4" s="34" t="s">
+      <c r="AK4" s="34" t="s">
         <v>68</v>
       </c>
+      <c r="AL4" s="34"/>
       <c r="AM4" s="34"/>
       <c r="AN4" s="34"/>
-      <c r="AO4" s="34"/>
-      <c r="AP4" s="16"/>
-      <c r="AQ4" s="23"/>
-      <c r="AR4" s="21"/>
-    </row>
-    <row r="5" spans="1:44" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="AO4" s="16"/>
+      <c r="AP4" s="23"/>
+      <c r="AQ4" s="21"/>
+    </row>
+    <row r="5" spans="1:43" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>71</v>
       </c>
@@ -1604,102 +1615,99 @@
         <v>85</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>180</v>
+        <v>86</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="R5" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="S5" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="T5" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="U5" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="V5" s="9" t="s">
-        <v>91</v>
+        <v>153</v>
       </c>
       <c r="W5" s="9" t="s">
-        <v>153</v>
+        <v>92</v>
       </c>
       <c r="X5" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="Y5" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Z5" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AA5" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AB5" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AC5" s="9" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="AD5" s="9" t="s">
-        <v>106</v>
+        <v>163</v>
       </c>
       <c r="AE5" s="9" t="s">
-        <v>163</v>
+        <v>102</v>
       </c>
       <c r="AF5" s="9" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="AG5" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AH5" s="9" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="AI5" s="9" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="AJ5" s="9" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="AK5" s="9" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="AL5" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AM5" s="9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AN5" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AO5" s="9" t="s">
-        <v>101</v>
+        <v>157</v>
       </c>
       <c r="AP5" s="9" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="AQ5" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="AR5" s="9" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C6" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" t="s">
         <v>109</v>
@@ -1737,123 +1745,1287 @@
       <c r="O6">
         <v>55</v>
       </c>
-      <c r="P6">
-        <v>60</v>
-      </c>
-      <c r="Q6" s="12">
+      <c r="P6" s="12">
         <v>0.02</v>
+      </c>
+      <c r="Q6">
+        <v>10</v>
       </c>
       <c r="R6">
         <v>10</v>
       </c>
-      <c r="S6">
+      <c r="S6" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T6" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U6" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V6" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="W6" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X6" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z6" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA6" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="AB6">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AD6" s="18">
+        <v>1</v>
+      </c>
+      <c r="AE6">
+        <v>200</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>142</v>
+      </c>
+      <c r="AG6">
+        <v>5</v>
+      </c>
+      <c r="AH6">
+        <v>200</v>
+      </c>
+      <c r="AI6" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ6">
+        <v>1</v>
+      </c>
+      <c r="AK6" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AL6" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="AM6" s="13">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN6" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="AO6" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP6" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ6" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="C9" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9" t="s">
+        <v>109</v>
+      </c>
+      <c r="F9" t="s">
+        <v>109</v>
+      </c>
+      <c r="G9" t="s">
+        <v>109</v>
+      </c>
+      <c r="H9" t="s">
+        <v>147</v>
+      </c>
+      <c r="I9" t="s">
+        <v>168</v>
+      </c>
+      <c r="J9" s="27">
+        <v>0</v>
+      </c>
+      <c r="K9" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L9" s="27">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="M9">
+        <v>3</v>
+      </c>
+      <c r="N9">
+        <v>60</v>
+      </c>
+      <c r="O9">
+        <v>60</v>
+      </c>
+      <c r="P9" s="27">
+        <v>0.02</v>
+      </c>
+      <c r="Q9">
         <v>10</v>
       </c>
-      <c r="T6" s="12">
+      <c r="R9">
+        <v>10</v>
+      </c>
+      <c r="S9" s="27">
         <v>0.03</v>
       </c>
-      <c r="U6" s="12">
+      <c r="T9" s="27">
         <v>0.01</v>
       </c>
-      <c r="V6" s="12">
+      <c r="U9" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="W6" s="12" t="s">
+      <c r="V9" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="X6" s="12">
+      <c r="W9" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="Y6" s="12">
-        <v>0</v>
-      </c>
-      <c r="Z6" t="s">
+      <c r="X9" s="27">
+        <v>0</v>
+      </c>
+      <c r="Y9" t="s">
         <v>112</v>
       </c>
-      <c r="AA6" s="2" t="s">
+      <c r="Z9" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="AB6" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="AC6">
+      <c r="AA9" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="AB9">
         <v>1</v>
       </c>
-      <c r="AD6" s="2" t="s">
+      <c r="AC9" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="AE6" s="18">
+      <c r="AD9" s="18">
         <v>1</v>
       </c>
-      <c r="AF6">
+      <c r="AE9">
         <v>200</v>
       </c>
-      <c r="AG6" t="s">
+      <c r="AF9" t="s">
         <v>142</v>
       </c>
-      <c r="AH6">
+      <c r="AG9">
         <v>5</v>
       </c>
-      <c r="AI6">
+      <c r="AH9">
         <v>200</v>
       </c>
-      <c r="AJ6" s="2" t="s">
+      <c r="AI9" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="AK6">
+      <c r="AJ9">
         <v>1</v>
       </c>
-      <c r="AL6" s="2" t="s">
+      <c r="AK9" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AM6" s="13">
+      <c r="AL9" s="13">
         <v>0.25</v>
       </c>
-      <c r="AN6" s="13">
+      <c r="AM9" s="13">
         <v>0.14499999999999999</v>
       </c>
-      <c r="AO6" s="13">
+      <c r="AN9" s="13">
         <v>0.05</v>
       </c>
-      <c r="AP6" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="AQ6" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="AR6" s="19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-    </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-    </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AO9" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP9" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ9" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>182</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="C10" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>171</v>
+      </c>
+      <c r="E10" t="s">
+        <v>171</v>
+      </c>
+      <c r="F10" t="s">
+        <v>109</v>
+      </c>
+      <c r="G10" t="s">
+        <v>109</v>
+      </c>
+      <c r="H10" t="s">
+        <v>147</v>
+      </c>
+      <c r="I10" t="s">
+        <v>168</v>
+      </c>
+      <c r="J10" s="27">
+        <v>0</v>
+      </c>
+      <c r="K10" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L10" s="27">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="M10">
+        <v>3</v>
+      </c>
+      <c r="N10">
+        <v>60</v>
+      </c>
+      <c r="O10">
+        <v>60</v>
+      </c>
+      <c r="P10" s="27">
+        <v>0.02</v>
+      </c>
+      <c r="Q10">
+        <v>10</v>
+      </c>
+      <c r="R10">
+        <v>10</v>
+      </c>
+      <c r="S10" s="27">
+        <v>0.03</v>
+      </c>
+      <c r="T10" s="27">
+        <v>0.01</v>
+      </c>
+      <c r="U10" s="27">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V10" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="W10" s="27">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X10" s="27">
+        <v>0</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z10" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA10" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="AB10">
+        <v>1</v>
+      </c>
+      <c r="AC10" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AD10" s="18">
+        <v>1</v>
+      </c>
+      <c r="AE10">
+        <v>200</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>142</v>
+      </c>
+      <c r="AG10">
+        <v>5</v>
+      </c>
+      <c r="AH10">
+        <v>200</v>
+      </c>
+      <c r="AI10" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ10">
+        <v>1</v>
+      </c>
+      <c r="AK10" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AL10" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="AM10" s="13">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN10" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="AO10" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP10" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ10" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>183</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="C11" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>172</v>
+      </c>
+      <c r="E11" t="s">
+        <v>172</v>
+      </c>
+      <c r="F11" t="s">
+        <v>109</v>
+      </c>
+      <c r="G11" t="s">
+        <v>109</v>
+      </c>
+      <c r="H11" t="s">
+        <v>147</v>
+      </c>
+      <c r="I11" t="s">
+        <v>168</v>
+      </c>
+      <c r="J11" s="27">
+        <v>0</v>
+      </c>
+      <c r="K11" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L11" s="27">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="M11">
+        <v>3</v>
+      </c>
+      <c r="N11">
+        <v>60</v>
+      </c>
+      <c r="O11">
+        <v>60</v>
+      </c>
+      <c r="P11" s="27">
+        <v>0.02</v>
+      </c>
+      <c r="Q11">
+        <v>10</v>
+      </c>
+      <c r="R11">
+        <v>10</v>
+      </c>
+      <c r="S11" s="27">
+        <v>0.03</v>
+      </c>
+      <c r="T11" s="27">
+        <v>0.01</v>
+      </c>
+      <c r="U11" s="27">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V11" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="W11" s="27">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X11" s="27">
+        <v>0</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z11" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA11" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="AB11">
+        <v>1</v>
+      </c>
+      <c r="AC11" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AD11" s="18">
+        <v>1</v>
+      </c>
+      <c r="AE11">
+        <v>200</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>142</v>
+      </c>
+      <c r="AG11">
+        <v>5</v>
+      </c>
+      <c r="AH11">
+        <v>200</v>
+      </c>
+      <c r="AI11" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ11">
+        <v>1</v>
+      </c>
+      <c r="AK11" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AL11" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="AM11" s="13">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN11" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="AO11" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP11" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ11" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="C12" s="27"/>
       <c r="D12" s="27"/>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-    </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="B14" s="26"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>184</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="C13" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" t="s">
+        <v>109</v>
+      </c>
+      <c r="F13" t="s">
+        <v>109</v>
+      </c>
+      <c r="G13" t="s">
+        <v>109</v>
+      </c>
+      <c r="H13" t="s">
+        <v>147</v>
+      </c>
+      <c r="I13" t="s">
+        <v>168</v>
+      </c>
+      <c r="J13" s="27">
+        <v>0</v>
+      </c>
+      <c r="K13" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L13" s="27">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="M13">
+        <v>3</v>
+      </c>
+      <c r="N13">
+        <v>65</v>
+      </c>
+      <c r="O13">
+        <v>55</v>
+      </c>
+      <c r="P13" s="27">
+        <v>0.02</v>
+      </c>
+      <c r="Q13">
+        <v>10</v>
+      </c>
+      <c r="R13">
+        <v>10</v>
+      </c>
+      <c r="S13" s="27">
+        <v>0.03</v>
+      </c>
+      <c r="T13" s="27">
+        <v>0.01</v>
+      </c>
+      <c r="U13" s="27">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V13" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="W13" s="27">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X13" s="27">
+        <v>0</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z13" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA13" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="AB13">
+        <v>1</v>
+      </c>
+      <c r="AC13" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AD13" s="18">
+        <v>1</v>
+      </c>
+      <c r="AE13">
+        <v>200</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>142</v>
+      </c>
+      <c r="AG13">
+        <v>5</v>
+      </c>
+      <c r="AH13">
+        <v>200</v>
+      </c>
+      <c r="AI13" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ13">
+        <v>1</v>
+      </c>
+      <c r="AK13" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AL13" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="AM13" s="13">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN13" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="AO13" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP13" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ13" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>185</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="C14" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>171</v>
+      </c>
+      <c r="E14" t="s">
+        <v>171</v>
+      </c>
+      <c r="F14" t="s">
+        <v>109</v>
+      </c>
+      <c r="G14" t="s">
+        <v>109</v>
+      </c>
+      <c r="H14" t="s">
+        <v>147</v>
+      </c>
+      <c r="I14" t="s">
+        <v>168</v>
+      </c>
+      <c r="J14" s="27">
+        <v>0</v>
+      </c>
+      <c r="K14" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L14" s="27">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="M14">
+        <v>3</v>
+      </c>
+      <c r="N14">
+        <v>65</v>
+      </c>
+      <c r="O14">
+        <v>55</v>
+      </c>
+      <c r="P14" s="27">
+        <v>0.02</v>
+      </c>
+      <c r="Q14">
+        <v>10</v>
+      </c>
+      <c r="R14">
+        <v>10</v>
+      </c>
+      <c r="S14" s="27">
+        <v>0.03</v>
+      </c>
+      <c r="T14" s="27">
+        <v>0.01</v>
+      </c>
+      <c r="U14" s="27">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V14" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="W14" s="27">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X14" s="27">
+        <v>0</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z14" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA14" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="AB14">
+        <v>1</v>
+      </c>
+      <c r="AC14" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AD14" s="18">
+        <v>1</v>
+      </c>
+      <c r="AE14">
+        <v>200</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>142</v>
+      </c>
+      <c r="AG14">
+        <v>5</v>
+      </c>
+      <c r="AH14">
+        <v>200</v>
+      </c>
+      <c r="AI14" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ14">
+        <v>1</v>
+      </c>
+      <c r="AK14" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AL14" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="AM14" s="13">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN14" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="AO14" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP14" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ14" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>186</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="C15" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>172</v>
+      </c>
+      <c r="E15" t="s">
+        <v>172</v>
+      </c>
+      <c r="F15" t="s">
+        <v>109</v>
+      </c>
+      <c r="G15" t="s">
+        <v>109</v>
+      </c>
+      <c r="H15" t="s">
+        <v>147</v>
+      </c>
+      <c r="I15" t="s">
+        <v>168</v>
+      </c>
+      <c r="J15" s="27">
+        <v>0</v>
+      </c>
+      <c r="K15" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L15" s="27">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="M15">
+        <v>3</v>
+      </c>
+      <c r="N15">
+        <v>65</v>
+      </c>
+      <c r="O15">
+        <v>55</v>
+      </c>
+      <c r="P15" s="27">
+        <v>0.02</v>
+      </c>
+      <c r="Q15">
+        <v>10</v>
+      </c>
+      <c r="R15">
+        <v>10</v>
+      </c>
+      <c r="S15" s="27">
+        <v>0.03</v>
+      </c>
+      <c r="T15" s="27">
+        <v>0.01</v>
+      </c>
+      <c r="U15" s="27">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V15" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="W15" s="27">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X15" s="27">
+        <v>0</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z15" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA15" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="AB15">
+        <v>1</v>
+      </c>
+      <c r="AC15" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AD15" s="18">
+        <v>1</v>
+      </c>
+      <c r="AE15">
+        <v>200</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>142</v>
+      </c>
+      <c r="AG15">
+        <v>5</v>
+      </c>
+      <c r="AH15">
+        <v>200</v>
+      </c>
+      <c r="AI15" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ15">
+        <v>1</v>
+      </c>
+      <c r="AK15" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AL15" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="AM15" s="13">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN15" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="AO15" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP15" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ15" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="C16" s="11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>187</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="C17" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17" t="s">
+        <v>109</v>
+      </c>
+      <c r="F17" t="s">
+        <v>109</v>
+      </c>
+      <c r="G17" t="s">
+        <v>109</v>
+      </c>
+      <c r="H17" t="s">
+        <v>147</v>
+      </c>
+      <c r="I17" t="s">
+        <v>168</v>
+      </c>
+      <c r="J17" s="27">
+        <v>0</v>
+      </c>
+      <c r="K17" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L17" s="27">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="M17">
+        <v>3</v>
+      </c>
+      <c r="N17">
+        <v>65</v>
+      </c>
+      <c r="O17">
+        <v>55</v>
+      </c>
+      <c r="P17" s="27">
+        <v>0.02</v>
+      </c>
+      <c r="Q17">
+        <v>10</v>
+      </c>
+      <c r="R17">
+        <v>10</v>
+      </c>
+      <c r="S17" s="27">
+        <v>0.03</v>
+      </c>
+      <c r="T17" s="27">
+        <v>0.01</v>
+      </c>
+      <c r="U17" s="27">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V17" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="W17" s="27">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X17" s="27">
+        <v>0</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z17" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA17" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="AB17">
+        <v>1</v>
+      </c>
+      <c r="AC17" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AD17" s="18">
+        <v>1</v>
+      </c>
+      <c r="AE17">
+        <v>200</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>142</v>
+      </c>
+      <c r="AG17">
+        <v>5</v>
+      </c>
+      <c r="AH17">
+        <v>200</v>
+      </c>
+      <c r="AI17" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ17">
+        <v>1</v>
+      </c>
+      <c r="AK17" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AL17" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="AM17" s="13">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN17" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="AO17" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP17" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ17" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>188</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="C18" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>171</v>
+      </c>
+      <c r="E18" t="s">
+        <v>171</v>
+      </c>
+      <c r="F18" t="s">
+        <v>109</v>
+      </c>
+      <c r="G18" t="s">
+        <v>109</v>
+      </c>
+      <c r="H18" t="s">
+        <v>147</v>
+      </c>
+      <c r="I18" t="s">
+        <v>168</v>
+      </c>
+      <c r="J18" s="27">
+        <v>0</v>
+      </c>
+      <c r="K18" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L18" s="27">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="M18">
+        <v>3</v>
+      </c>
+      <c r="N18">
+        <v>65</v>
+      </c>
+      <c r="O18">
+        <v>55</v>
+      </c>
+      <c r="P18" s="27">
+        <v>0.02</v>
+      </c>
+      <c r="Q18">
+        <v>10</v>
+      </c>
+      <c r="R18">
+        <v>10</v>
+      </c>
+      <c r="S18" s="27">
+        <v>0.03</v>
+      </c>
+      <c r="T18" s="27">
+        <v>0.01</v>
+      </c>
+      <c r="U18" s="27">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V18" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="W18" s="27">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X18" s="27">
+        <v>0</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z18" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA18" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="AB18">
+        <v>1</v>
+      </c>
+      <c r="AC18" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AD18" s="18">
+        <v>1</v>
+      </c>
+      <c r="AE18">
+        <v>200</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>142</v>
+      </c>
+      <c r="AG18">
+        <v>5</v>
+      </c>
+      <c r="AH18">
+        <v>200</v>
+      </c>
+      <c r="AI18" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ18">
+        <v>1</v>
+      </c>
+      <c r="AK18" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AL18" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="AM18" s="13">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN18" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="AO18" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP18" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ18" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>189</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="C19" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>172</v>
+      </c>
+      <c r="E19" t="s">
+        <v>172</v>
+      </c>
+      <c r="F19" t="s">
+        <v>109</v>
+      </c>
+      <c r="G19" t="s">
+        <v>109</v>
+      </c>
+      <c r="H19" t="s">
+        <v>147</v>
+      </c>
+      <c r="I19" t="s">
+        <v>168</v>
+      </c>
+      <c r="J19" s="27">
+        <v>0</v>
+      </c>
+      <c r="K19" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L19" s="27">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="M19">
+        <v>3</v>
+      </c>
+      <c r="N19">
+        <v>65</v>
+      </c>
+      <c r="O19">
+        <v>55</v>
+      </c>
+      <c r="P19" s="27">
+        <v>0.02</v>
+      </c>
+      <c r="Q19">
+        <v>10</v>
+      </c>
+      <c r="R19">
+        <v>10</v>
+      </c>
+      <c r="S19" s="27">
+        <v>0.03</v>
+      </c>
+      <c r="T19" s="27">
+        <v>0.01</v>
+      </c>
+      <c r="U19" s="27">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V19" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="W19" s="27">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X19" s="27">
+        <v>0</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z19" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA19" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="AB19">
+        <v>1</v>
+      </c>
+      <c r="AC19" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AD19" s="18">
+        <v>1</v>
+      </c>
+      <c r="AE19">
+        <v>200</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>142</v>
+      </c>
+      <c r="AG19">
+        <v>5</v>
+      </c>
+      <c r="AH19">
+        <v>200</v>
+      </c>
+      <c r="AI19" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ19">
+        <v>1</v>
+      </c>
+      <c r="AK19" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AL19" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="AM19" s="13">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN19" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="AO19" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP19" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ19" s="19" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="AD4:AF4"/>
-    <mergeCell ref="L4:S4"/>
-    <mergeCell ref="T4:V4"/>
-    <mergeCell ref="AA4:AC4"/>
-    <mergeCell ref="AL4:AO4"/>
-    <mergeCell ref="W4:Y4"/>
+    <mergeCell ref="AC4:AE4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="AK4:AN4"/>
+    <mergeCell ref="V4:X4"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="F4:G4"/>
@@ -1861,78 +3033,78 @@
     <mergeCell ref="J4:K4"/>
   </mergeCells>
   <dataValidations count="20">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI6 AI9:AI11 AI13:AI15 AI17:AI19">
       <formula1>"MA,EAA"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA6 AA9:AA11 AA13:AA15 AA17:AA19">
       <formula1>"cd,cp,sl"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z6 Z9:Z11 Z13:Z15 Z17:Z19">
       <formula1>"open,closed"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK6 AK9:AK11 AK13:AK15 AK17:AK19">
       <formula1>ConPolicy</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6 C6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6 C6 K9:K11 C9:C11 K13:K15 K17:K19 C13:C19">
       <formula1>"TRUE,FALSE"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer 55 to 65, please" sqref="N6">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer 55 to 65, please" sqref="N6 N9:N11 N17:N19 N13:N15">
       <formula1>55</formula1>
       <formula2>65</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="Q6 U6">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="P6 T6 P9:P11 T9:T11 P13:P15 T13:T15 P17:P19 T17:T19">
       <formula1>0</formula1>
       <formula2>0.1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="R6:S6">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="Q6:R6 Q9:R11 Q13:R15 Q17:R19">
       <formula1>0</formula1>
       <formula2>15</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="T6 X6 V6">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="S6 W6 U6 S9:S11 W9:W11 U9:U11 S13:S15 W13:W15 U13:U15 S17:S19 W17:W19 U17:U19">
       <formula1>0</formula1>
       <formula2>0.2</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AC6">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AB6 AB9:AB11 AB13:AB15 AB17:AB19">
       <formula1>0</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AM6:AN6">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AL6:AM6 AL9:AM11 AL13:AM15 AL17:AM19">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AO6">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AN6 AN9:AN11 AN13:AN15 AN17:AN19">
       <formula1>0</formula1>
       <formula2>0.3</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="Y6">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="X6 X9:X11 X13:X15 X17:X19">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AH6">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AG6 AG9:AG11 AG13:AG15 AG17:AG19">
       <formula1>1</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI6">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH6 AH9:AH11 AH13:AH15 AH17:AH19">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK6">
+    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ6 AJ9:AJ11 AJ13:AJ15 AJ17:AJ19">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="W6"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP6:AR6">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="V6 V9:V11 V13:V15 V17:V19"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO6:AQ6 AO9:AQ11 AO13:AQ15 AO17:AQ19">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC6 AC9:AC11 AC13:AC15 AC17:AC19">
       <formula1>"MA,AL,AL_pct"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE6">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD6 AD9:AD11 AD13:AD15 AD17:AD19">
       <formula1>0</formula1>
       <formula2>1.5</formula2>
     </dataValidation>
@@ -1946,19 +3118,19 @@
           <x14:formula1>
             <xm:f>DropDowns!$A$33:$A$37</xm:f>
           </x14:formula1>
-          <xm:sqref>H6</xm:sqref>
+          <xm:sqref>H6 H9:H11 H13:H15 H17:H19</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$40:$A$42</xm:f>
           </x14:formula1>
-          <xm:sqref>I6</xm:sqref>
+          <xm:sqref>I6 I9:I11 I13:I15 I17:I19</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$20:$A$25</xm:f>
           </x14:formula1>
-          <xm:sqref>D6:G6</xm:sqref>
+          <xm:sqref>D6:G6 D13:G15 D9:G11 D17:G19</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2120,8 +3292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2159,10 +3331,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="B3">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>6</v>
@@ -2321,22 +3493,22 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -2449,7 +3621,7 @@
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B2">
         <v>2.7E-2</v>
@@ -2457,7 +3629,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B3">
         <v>0.4</v>
@@ -2465,10 +3637,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
check AL issues in young and underfunded plans
</commit_message>
<xml_diff>
--- a/IO_Dev/RunControl_Dev.xlsx
+++ b/IO_Dev/RunControl_Dev.xlsx
@@ -801,7 +801,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -810,16 +816,10 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1323,13 +1323,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR19"/>
+  <dimension ref="A1:AR18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="E25" sqref="E25"/>
+      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1502,60 +1502,60 @@
       </c>
     </row>
     <row r="4" spans="1:44" s="8" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="33" t="s">
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="33"/>
-      <c r="F4" s="34" t="s">
+      <c r="E4" s="29"/>
+      <c r="F4" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="34"/>
-      <c r="H4" s="29" t="s">
+      <c r="G4" s="30"/>
+      <c r="H4" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="I4" s="29"/>
-      <c r="J4" s="30" t="s">
+      <c r="I4" s="31"/>
+      <c r="J4" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="K4" s="30"/>
-      <c r="L4" s="29" t="s">
+      <c r="K4" s="32"/>
+      <c r="L4" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="29"/>
-      <c r="S4" s="29"/>
-      <c r="T4" s="30" t="s">
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="31"/>
+      <c r="T4" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="U4" s="30"/>
-      <c r="V4" s="30"/>
-      <c r="W4" s="28" t="s">
+      <c r="U4" s="32"/>
+      <c r="V4" s="32"/>
+      <c r="W4" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="X4" s="28"/>
-      <c r="Y4" s="28"/>
+      <c r="X4" s="33"/>
+      <c r="Y4" s="33"/>
       <c r="Z4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AA4" s="31" t="s">
+      <c r="AA4" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="AB4" s="31"/>
-      <c r="AC4" s="31"/>
-      <c r="AD4" s="28" t="s">
+      <c r="AB4" s="28"/>
+      <c r="AC4" s="28"/>
+      <c r="AD4" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="AE4" s="28"/>
-      <c r="AF4" s="28"/>
+      <c r="AE4" s="33"/>
+      <c r="AF4" s="33"/>
       <c r="AG4" s="22" t="s">
         <v>70</v>
       </c>
@@ -1563,12 +1563,12 @@
       <c r="AI4" s="22"/>
       <c r="AJ4" s="22"/>
       <c r="AK4" s="22"/>
-      <c r="AL4" s="32" t="s">
+      <c r="AL4" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="AM4" s="32"/>
-      <c r="AN4" s="32"/>
-      <c r="AO4" s="32"/>
+      <c r="AM4" s="34"/>
+      <c r="AN4" s="34"/>
+      <c r="AO4" s="34"/>
       <c r="AP4" s="16"/>
       <c r="AQ4" s="23"/>
       <c r="AR4" s="21"/>
@@ -1715,7 +1715,7 @@
         <v>175</v>
       </c>
       <c r="C6" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
         <v>109</v>
@@ -1739,7 +1739,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6" s="12">
         <v>2.1999999999999999E-2</v>
@@ -1841,9 +1841,143 @@
         <v>0</v>
       </c>
     </row>
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="C8" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" t="s">
+        <v>109</v>
+      </c>
+      <c r="F8" t="s">
+        <v>109</v>
+      </c>
+      <c r="G8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H8" t="s">
+        <v>147</v>
+      </c>
+      <c r="I8" t="s">
+        <v>168</v>
+      </c>
+      <c r="J8" s="27">
+        <v>0</v>
+      </c>
+      <c r="K8" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L8" s="27">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="M8">
+        <v>3</v>
+      </c>
+      <c r="N8">
+        <v>65</v>
+      </c>
+      <c r="O8">
+        <v>65</v>
+      </c>
+      <c r="P8">
+        <v>65</v>
+      </c>
+      <c r="Q8" s="27">
+        <v>0.02</v>
+      </c>
+      <c r="R8">
+        <v>10</v>
+      </c>
+      <c r="S8">
+        <v>10</v>
+      </c>
+      <c r="T8" s="27">
+        <v>0.03</v>
+      </c>
+      <c r="U8" s="27">
+        <v>0.01</v>
+      </c>
+      <c r="V8" s="27">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="W8" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="X8" s="27">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="Y8" s="27">
+        <v>0</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA8" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB8" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="AC8">
+        <v>1</v>
+      </c>
+      <c r="AD8" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AE8" s="18">
+        <v>1</v>
+      </c>
+      <c r="AF8">
+        <v>200</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>142</v>
+      </c>
+      <c r="AH8">
+        <v>5</v>
+      </c>
+      <c r="AI8">
+        <v>200</v>
+      </c>
+      <c r="AJ8" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AK8">
+        <v>1</v>
+      </c>
+      <c r="AL8" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AM8" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="AN8" s="13">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AO8" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="AP8" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ8" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR8" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>175</v>
@@ -1852,10 +1986,10 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>109</v>
+        <v>171</v>
       </c>
       <c r="E9" t="s">
-        <v>109</v>
+        <v>171</v>
       </c>
       <c r="F9" t="s">
         <v>109</v>
@@ -1977,7 +2111,7 @@
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B10" s="20" t="s">
         <v>175</v>
@@ -1986,10 +2120,10 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E10" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F10" t="s">
         <v>109</v>
@@ -2110,146 +2244,146 @@
       </c>
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>183</v>
-      </c>
-      <c r="B11" s="20" t="s">
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+    </row>
+    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>184</v>
+      </c>
+      <c r="B12" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="C11" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" t="s">
-        <v>172</v>
-      </c>
-      <c r="E11" t="s">
-        <v>172</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="C12" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
         <v>109</v>
       </c>
-      <c r="G11" t="s">
+      <c r="E12" t="s">
         <v>109</v>
       </c>
-      <c r="H11" t="s">
+      <c r="F12" t="s">
+        <v>109</v>
+      </c>
+      <c r="G12" t="s">
+        <v>109</v>
+      </c>
+      <c r="H12" t="s">
         <v>147</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I12" t="s">
         <v>168</v>
       </c>
-      <c r="J11" s="27">
-        <v>0</v>
-      </c>
-      <c r="K11" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="L11" s="27">
+      <c r="J12" s="27">
+        <v>0</v>
+      </c>
+      <c r="K12" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L12" s="27">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="M11">
+      <c r="M12">
         <v>3</v>
       </c>
-      <c r="N11">
+      <c r="N12">
         <v>65</v>
       </c>
-      <c r="O11">
+      <c r="O12">
+        <v>55</v>
+      </c>
+      <c r="P12">
         <v>65</v>
       </c>
-      <c r="P11">
-        <v>65</v>
-      </c>
-      <c r="Q11" s="27">
+      <c r="Q12" s="27">
         <v>0.02</v>
       </c>
-      <c r="R11">
+      <c r="R12">
         <v>10</v>
       </c>
-      <c r="S11">
+      <c r="S12">
         <v>10</v>
       </c>
-      <c r="T11" s="27">
+      <c r="T12" s="27">
         <v>0.03</v>
       </c>
-      <c r="U11" s="27">
+      <c r="U12" s="27">
         <v>0.01</v>
       </c>
-      <c r="V11" s="27">
+      <c r="V12" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="W11" s="27" t="s">
+      <c r="W12" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="X11" s="27">
+      <c r="X12" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="Y11" s="27">
-        <v>0</v>
-      </c>
-      <c r="Z11" t="s">
+      <c r="Y12" s="27">
+        <v>0</v>
+      </c>
+      <c r="Z12" t="s">
         <v>112</v>
       </c>
-      <c r="AA11" s="2" t="s">
+      <c r="AA12" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="AB11" s="2" t="s">
+      <c r="AB12" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="AC11">
+      <c r="AC12">
         <v>1</v>
       </c>
-      <c r="AD11" s="2" t="s">
+      <c r="AD12" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="AE11" s="18">
+      <c r="AE12" s="18">
         <v>1</v>
       </c>
-      <c r="AF11">
+      <c r="AF12">
         <v>200</v>
       </c>
-      <c r="AG11" t="s">
+      <c r="AG12" t="s">
         <v>142</v>
       </c>
-      <c r="AH11">
+      <c r="AH12">
         <v>5</v>
       </c>
-      <c r="AI11">
+      <c r="AI12">
         <v>200</v>
       </c>
-      <c r="AJ11" s="2" t="s">
+      <c r="AJ12" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="AK11">
+      <c r="AK12">
         <v>1</v>
       </c>
-      <c r="AL11" s="2" t="s">
+      <c r="AL12" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AM11" s="13">
+      <c r="AM12" s="13">
         <v>0.25</v>
       </c>
-      <c r="AN11" s="13">
+      <c r="AN12" s="13">
         <v>0.14499999999999999</v>
       </c>
-      <c r="AO11" s="13">
+      <c r="AO12" s="13">
         <v>0.05</v>
       </c>
-      <c r="AP11" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="AQ11" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="AR11" s="19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
+      <c r="AP12" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ12" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR12" s="19" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B13" s="20" t="s">
         <v>175</v>
@@ -2258,10 +2392,10 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>109</v>
+        <v>171</v>
       </c>
       <c r="E13" t="s">
-        <v>109</v>
+        <v>171</v>
       </c>
       <c r="F13" t="s">
         <v>109</v>
@@ -2383,7 +2517,7 @@
     </row>
     <row r="14" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B14" s="20" t="s">
         <v>175</v>
@@ -2392,10 +2526,10 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E14" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F14" t="s">
         <v>109</v>
@@ -2516,157 +2650,157 @@
       </c>
     </row>
     <row r="15" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>186</v>
-      </c>
-      <c r="B15" s="20" t="s">
+      <c r="C15" s="11"/>
+    </row>
+    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>187</v>
+      </c>
+      <c r="B16" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="C15" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" t="s">
-        <v>172</v>
-      </c>
-      <c r="E15" t="s">
-        <v>172</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="C16" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
         <v>109</v>
       </c>
-      <c r="G15" t="s">
+      <c r="E16" t="s">
         <v>109</v>
       </c>
-      <c r="H15" t="s">
+      <c r="F16" t="s">
+        <v>109</v>
+      </c>
+      <c r="G16" t="s">
+        <v>109</v>
+      </c>
+      <c r="H16" t="s">
         <v>147</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I16" t="s">
         <v>168</v>
       </c>
-      <c r="J15" s="27">
-        <v>0</v>
-      </c>
-      <c r="K15" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="L15" s="27">
+      <c r="J16" s="27">
+        <v>0</v>
+      </c>
+      <c r="K16" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L16" s="27">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="M15">
+      <c r="M16">
         <v>3</v>
       </c>
-      <c r="N15">
+      <c r="N16">
         <v>65</v>
       </c>
-      <c r="O15">
+      <c r="O16">
         <v>55</v>
       </c>
-      <c r="P15">
+      <c r="P16">
         <v>65</v>
       </c>
-      <c r="Q15" s="27">
+      <c r="Q16" s="27">
         <v>0.02</v>
       </c>
-      <c r="R15">
+      <c r="R16">
         <v>10</v>
       </c>
-      <c r="S15">
+      <c r="S16">
         <v>10</v>
       </c>
-      <c r="T15" s="27">
+      <c r="T16" s="27">
         <v>0.03</v>
       </c>
-      <c r="U15" s="27">
+      <c r="U16" s="27">
         <v>0.01</v>
       </c>
-      <c r="V15" s="27">
+      <c r="V16" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="W15" s="27" t="s">
+      <c r="W16" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="X15" s="27">
+      <c r="X16" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="Y15" s="27">
-        <v>0</v>
-      </c>
-      <c r="Z15" t="s">
+      <c r="Y16" s="27">
+        <v>0</v>
+      </c>
+      <c r="Z16" t="s">
         <v>112</v>
       </c>
-      <c r="AA15" s="2" t="s">
+      <c r="AA16" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="AB15" s="2" t="s">
+      <c r="AB16" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="AC15">
+      <c r="AC16">
         <v>1</v>
       </c>
-      <c r="AD15" s="2" t="s">
+      <c r="AD16" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="AE15" s="18">
+      <c r="AE16" s="18">
         <v>1</v>
       </c>
-      <c r="AF15">
+      <c r="AF16">
         <v>200</v>
       </c>
-      <c r="AG15" t="s">
+      <c r="AG16" t="s">
         <v>142</v>
       </c>
-      <c r="AH15">
+      <c r="AH16">
         <v>5</v>
       </c>
-      <c r="AI15">
+      <c r="AI16">
         <v>200</v>
       </c>
-      <c r="AJ15" s="2" t="s">
+      <c r="AJ16" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="AK15">
+      <c r="AK16">
         <v>1</v>
       </c>
-      <c r="AL15" s="2" t="s">
+      <c r="AL16" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AM15" s="13">
+      <c r="AM16" s="13">
         <v>0.25</v>
       </c>
-      <c r="AN15" s="13">
+      <c r="AN16" s="13">
         <v>0.14499999999999999</v>
       </c>
-      <c r="AO15" s="13">
+      <c r="AO16" s="13">
         <v>0.05</v>
       </c>
-      <c r="AP15" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="AQ15" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="AR15" s="19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="C16" s="11"/>
+      <c r="AP16" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ16" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR16" s="19" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B17" s="20" t="s">
         <v>175</v>
       </c>
       <c r="C17" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>109</v>
+        <v>171</v>
       </c>
       <c r="E17" t="s">
-        <v>109</v>
+        <v>171</v>
       </c>
       <c r="F17" t="s">
         <v>109</v>
@@ -2788,19 +2922,19 @@
     </row>
     <row r="18" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B18" s="20" t="s">
         <v>175</v>
       </c>
       <c r="C18" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E18" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F18" t="s">
         <v>109</v>
@@ -2920,227 +3054,93 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>189</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>175</v>
-      </c>
-      <c r="C19" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>172</v>
-      </c>
-      <c r="E19" t="s">
-        <v>172</v>
-      </c>
-      <c r="F19" t="s">
-        <v>109</v>
-      </c>
-      <c r="G19" t="s">
-        <v>109</v>
-      </c>
-      <c r="H19" t="s">
-        <v>147</v>
-      </c>
-      <c r="I19" t="s">
-        <v>168</v>
-      </c>
-      <c r="J19" s="27">
-        <v>0</v>
-      </c>
-      <c r="K19" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="L19" s="27">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="M19">
-        <v>3</v>
-      </c>
-      <c r="N19">
-        <v>65</v>
-      </c>
-      <c r="O19">
-        <v>55</v>
-      </c>
-      <c r="P19">
-        <v>65</v>
-      </c>
-      <c r="Q19" s="27">
-        <v>0.02</v>
-      </c>
-      <c r="R19">
-        <v>10</v>
-      </c>
-      <c r="S19">
-        <v>10</v>
-      </c>
-      <c r="T19" s="27">
-        <v>0.03</v>
-      </c>
-      <c r="U19" s="27">
-        <v>0.01</v>
-      </c>
-      <c r="V19" s="27">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="W19" s="27" t="s">
-        <v>156</v>
-      </c>
-      <c r="X19" s="27">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="Y19" s="27">
-        <v>0</v>
-      </c>
-      <c r="Z19" t="s">
-        <v>112</v>
-      </c>
-      <c r="AA19" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="AB19" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="AC19">
-        <v>1</v>
-      </c>
-      <c r="AD19" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="AE19" s="18">
-        <v>1</v>
-      </c>
-      <c r="AF19">
-        <v>200</v>
-      </c>
-      <c r="AG19" t="s">
-        <v>142</v>
-      </c>
-      <c r="AH19">
-        <v>5</v>
-      </c>
-      <c r="AI19">
-        <v>200</v>
-      </c>
-      <c r="AJ19" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AK19">
-        <v>1</v>
-      </c>
-      <c r="AL19" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="AM19" s="13">
-        <v>0.25</v>
-      </c>
-      <c r="AN19" s="13">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="AO19" s="13">
-        <v>0.05</v>
-      </c>
-      <c r="AP19" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="AQ19" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="AR19" s="19" t="b">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
     <mergeCell ref="AD4:AF4"/>
     <mergeCell ref="L4:S4"/>
     <mergeCell ref="T4:V4"/>
     <mergeCell ref="AA4:AC4"/>
     <mergeCell ref="AL4:AO4"/>
     <mergeCell ref="W4:Y4"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <dataValidations count="20">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ6 AJ9:AJ11 AJ13:AJ15 AJ17:AJ19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ6 AJ8:AJ10 AJ12:AJ14 AJ16:AJ18">
       <formula1>"MA,EAA"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB6 AB9:AB11 AB13:AB15 AB17:AB19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB6 AB8:AB10 AB12:AB14 AB16:AB18">
       <formula1>"cd,cp,sl"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA6 AA9:AA11 AA13:AA15 AA17:AA19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA6 AA8:AA10 AA12:AA14 AA16:AA18">
       <formula1>"open,closed"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL6 AL9:AL11 AL13:AL15 AL17:AL19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL6 AL8:AL10 AL12:AL14 AL16:AL18">
       <formula1>ConPolicy</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6 C6 K9:K11 C9:C11 K13:K15 K17:K19 C13:C19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6 C6 K8:K10 C12:C18 K12:K14 K16:K18 C8:C10">
       <formula1>"TRUE,FALSE"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer 55 to 65, please" sqref="N6 N17:N19 N13:N15 N9:P11">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer 55 to 65, please" sqref="N6 N16:N18 N12:N14 N8:O10 P8:P18">
       <formula1>55</formula1>
       <formula2>65</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="Q6 U6 Q9:Q11 U9:U11 Q13:Q15 U13:U15 Q17:Q19 U17:U19">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="Q6 U6 Q8:Q10 U8:U10 Q12:Q14 U12:U14 Q16:Q18 U16:U18">
       <formula1>0</formula1>
       <formula2>0.1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="R6:S6 R9:S11 R13:S15 R17:S19">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="R6:S6 R8:S10 R12:S14 R16:S18">
       <formula1>0</formula1>
       <formula2>15</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="T6 X6 V6 T9:T11 X9:X11 V9:V11 T13:T15 X13:X15 V13:V15 T17:T19 X17:X19 V17:V19">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="T6 X6 V6 T8:T10 X8:X10 V8:V10 T12:T14 X12:X14 V12:V14 T16:T18 X16:X18 V16:V18">
       <formula1>0</formula1>
       <formula2>0.2</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AC6 AC9:AC11 AC13:AC15 AC17:AC19">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AC6 AC8:AC10 AC12:AC14 AC16:AC18">
       <formula1>0</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AM6:AN6 AM9:AN11 AM13:AN15 AM17:AN19">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AM6:AN6 AM8:AN10 AM12:AN14 AM16:AN18">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AO6 AO9:AO11 AO13:AO15 AO17:AO19">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AO6 AO8:AO10 AO12:AO14 AO16:AO18">
       <formula1>0</formula1>
       <formula2>0.3</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="Y6 Y9:Y11 Y13:Y15 Y17:Y19">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="Y6 Y8:Y10 Y12:Y14 Y16:Y18">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AH6 AH9:AH11 AH13:AH15 AH17:AH19">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AH6 AH8:AH10 AH12:AH14 AH16:AH18">
       <formula1>1</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI6 AI9:AI11 AI13:AI15 AI17:AI19">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI6 AI8:AI10 AI12:AI14 AI16:AI18">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK6 AK9:AK11 AK13:AK15 AK17:AK19">
+    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK6 AK8:AK10 AK12:AK14 AK16:AK18">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="W6 W9:W11 W13:W15 W17:W19"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP6:AR6 AP9:AR11 AP13:AR15 AP17:AR19">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="W6 W8:W10 W12:W14 W16:W18"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP6:AR6 AP8:AR10 AP12:AR14 AP16:AR18">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD6 AD9:AD11 AD13:AD15 AD17:AD19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD6 AD8:AD10 AD12:AD14 AD16:AD18">
       <formula1>"MA,AL,AL_pct"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE6 AE9:AE11 AE13:AE15 AE17:AE19">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE6 AE8:AE10 AE12:AE14 AE16:AE18">
       <formula1>0</formula1>
       <formula2>1.5</formula2>
     </dataValidation>
@@ -3154,19 +3154,19 @@
           <x14:formula1>
             <xm:f>DropDowns!$A$33:$A$37</xm:f>
           </x14:formula1>
-          <xm:sqref>H6 H9:H11 H13:H15 H17:H19</xm:sqref>
+          <xm:sqref>H6 H8:H10 H12:H14 H16:H18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$40:$A$42</xm:f>
           </x14:formula1>
-          <xm:sqref>I6 I9:I11 I13:I15 I17:I19</xm:sqref>
+          <xm:sqref>I6 I8:I10 I12:I14 I16:I18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$20:$A$25</xm:f>
           </x14:formula1>
-          <xm:sqref>D6:G6 D13:G15 D9:G11 D17:G19</xm:sqref>
+          <xm:sqref>D6:G6 D12:G14 D8:G10 D16:G18</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3329,7 +3329,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3367,7 +3367,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>10</v>

</xml_diff>

<commit_message>
Solve the 0 AL problem by converting NAs in Bx to 0
Still not clear why this happens
</commit_message>
<xml_diff>
--- a/IO_Dev/RunControl_Dev.xlsx
+++ b/IO_Dev/RunControl_Dev.xlsx
@@ -801,13 +801,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -816,10 +810,16 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1329,7 +1329,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
+      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1502,60 +1502,60 @@
       </c>
     </row>
     <row r="4" spans="1:44" s="8" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="29" t="s">
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="29"/>
-      <c r="F4" s="30" t="s">
+      <c r="E4" s="33"/>
+      <c r="F4" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="30"/>
-      <c r="H4" s="31" t="s">
+      <c r="G4" s="34"/>
+      <c r="H4" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="I4" s="31"/>
-      <c r="J4" s="32" t="s">
+      <c r="I4" s="29"/>
+      <c r="J4" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="K4" s="32"/>
-      <c r="L4" s="31" t="s">
+      <c r="K4" s="30"/>
+      <c r="L4" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="M4" s="31"/>
-      <c r="N4" s="31"/>
-      <c r="O4" s="31"/>
-      <c r="P4" s="31"/>
-      <c r="Q4" s="31"/>
-      <c r="R4" s="31"/>
-      <c r="S4" s="31"/>
-      <c r="T4" s="32" t="s">
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="29"/>
+      <c r="T4" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="U4" s="32"/>
-      <c r="V4" s="32"/>
-      <c r="W4" s="33" t="s">
+      <c r="U4" s="30"/>
+      <c r="V4" s="30"/>
+      <c r="W4" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="X4" s="33"/>
-      <c r="Y4" s="33"/>
+      <c r="X4" s="28"/>
+      <c r="Y4" s="28"/>
       <c r="Z4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AA4" s="28" t="s">
+      <c r="AA4" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="AB4" s="28"/>
-      <c r="AC4" s="28"/>
-      <c r="AD4" s="33" t="s">
+      <c r="AB4" s="31"/>
+      <c r="AC4" s="31"/>
+      <c r="AD4" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="AE4" s="33"/>
-      <c r="AF4" s="33"/>
+      <c r="AE4" s="28"/>
+      <c r="AF4" s="28"/>
       <c r="AG4" s="22" t="s">
         <v>70</v>
       </c>
@@ -1563,12 +1563,12 @@
       <c r="AI4" s="22"/>
       <c r="AJ4" s="22"/>
       <c r="AK4" s="22"/>
-      <c r="AL4" s="34" t="s">
+      <c r="AL4" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="AM4" s="34"/>
-      <c r="AN4" s="34"/>
-      <c r="AO4" s="34"/>
+      <c r="AM4" s="32"/>
+      <c r="AN4" s="32"/>
+      <c r="AO4" s="32"/>
       <c r="AP4" s="16"/>
       <c r="AQ4" s="23"/>
       <c r="AR4" s="21"/>
@@ -3056,17 +3056,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
     <mergeCell ref="AD4:AF4"/>
     <mergeCell ref="L4:S4"/>
     <mergeCell ref="T4:V4"/>
     <mergeCell ref="AA4:AC4"/>
     <mergeCell ref="AL4:AO4"/>
     <mergeCell ref="W4:Y4"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <dataValidations count="20">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ6 AJ8:AJ10 AJ12:AJ14 AJ16:AJ18">
@@ -3367,7 +3367,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="B3">
         <v>10</v>

</xml_diff>

<commit_message>
Cleaning up for MRA.
</commit_message>
<xml_diff>
--- a/IO_Dev/RunControl_Dev.xlsx
+++ b/IO_Dev/RunControl_Dev.xlsx
@@ -25,7 +25,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Returns!$A$3:$D$12</definedName>
     <definedName name="ConPolicy">DropDowns!$A$12:$A$14</definedName>
   </definedNames>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -801,13 +801,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -816,10 +810,16 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1326,10 +1326,10 @@
   <dimension ref="A1:AR19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="J6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="P24" sqref="P24"/>
+      <selection pane="bottomRight" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1502,60 +1502,60 @@
       </c>
     </row>
     <row r="4" spans="1:44" s="8" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="29" t="s">
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="29"/>
-      <c r="F4" s="30" t="s">
+      <c r="E4" s="33"/>
+      <c r="F4" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="30"/>
-      <c r="H4" s="31" t="s">
+      <c r="G4" s="34"/>
+      <c r="H4" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="I4" s="31"/>
-      <c r="J4" s="32" t="s">
+      <c r="I4" s="29"/>
+      <c r="J4" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="K4" s="32"/>
-      <c r="L4" s="31" t="s">
+      <c r="K4" s="30"/>
+      <c r="L4" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="M4" s="31"/>
-      <c r="N4" s="31"/>
-      <c r="O4" s="31"/>
-      <c r="P4" s="31"/>
-      <c r="Q4" s="31"/>
-      <c r="R4" s="31"/>
-      <c r="S4" s="31"/>
-      <c r="T4" s="32" t="s">
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="29"/>
+      <c r="T4" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="U4" s="32"/>
-      <c r="V4" s="32"/>
-      <c r="W4" s="33" t="s">
+      <c r="U4" s="30"/>
+      <c r="V4" s="30"/>
+      <c r="W4" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="X4" s="33"/>
-      <c r="Y4" s="33"/>
+      <c r="X4" s="28"/>
+      <c r="Y4" s="28"/>
       <c r="Z4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AA4" s="28" t="s">
+      <c r="AA4" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="AB4" s="28"/>
-      <c r="AC4" s="28"/>
-      <c r="AD4" s="33" t="s">
+      <c r="AB4" s="31"/>
+      <c r="AC4" s="31"/>
+      <c r="AD4" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="AE4" s="33"/>
-      <c r="AF4" s="33"/>
+      <c r="AE4" s="28"/>
+      <c r="AF4" s="28"/>
       <c r="AG4" s="22" t="s">
         <v>70</v>
       </c>
@@ -1563,12 +1563,12 @@
       <c r="AI4" s="22"/>
       <c r="AJ4" s="22"/>
       <c r="AK4" s="22"/>
-      <c r="AL4" s="34" t="s">
+      <c r="AL4" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="AM4" s="34"/>
-      <c r="AN4" s="34"/>
-      <c r="AO4" s="34"/>
+      <c r="AM4" s="32"/>
+      <c r="AN4" s="32"/>
+      <c r="AO4" s="32"/>
       <c r="AP4" s="16"/>
       <c r="AQ4" s="23"/>
       <c r="AR4" s="21"/>
@@ -3056,17 +3056,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
     <mergeCell ref="AD4:AF4"/>
     <mergeCell ref="L4:S4"/>
     <mergeCell ref="T4:V4"/>
     <mergeCell ref="AA4:AC4"/>
     <mergeCell ref="AL4:AO4"/>
     <mergeCell ref="W4:Y4"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <dataValidations count="20">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ6 AJ9:AJ11 AJ13:AJ15 AJ17:AJ19">

</xml_diff>

<commit_message>
make new prototypes internally consistent
</commit_message>
<xml_diff>
--- a/IO_Dev/RunControl_Dev.xlsx
+++ b/IO_Dev/RunControl_Dev.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\PenSim-Projects\Model_Main\IO_Dev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Model_Main\IO_Dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="7230" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="7230" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Returns!$A$3:$D$12</definedName>
     <definedName name="ConPolicy">DropDowns!$A$12:$A$14</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="202">
   <si>
     <t>Sheet #</t>
   </si>
@@ -633,12 +633,15 @@
   </si>
   <si>
     <t>n_init_actives</t>
+  </si>
+  <si>
+    <t>startingSal.growth</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
@@ -695,7 +698,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -762,6 +765,12 @@
         <bgColor rgb="FFC5E0B4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFF2CC"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -778,7 +787,7 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -840,7 +849,13 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -849,16 +864,13 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1362,13 +1374,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AV19"/>
+  <dimension ref="A1:AW19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomRight" activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1384,30 +1396,32 @@
     <col min="14" max="15" width="13.140625" customWidth="1"/>
     <col min="16" max="20" width="9.28515625" customWidth="1"/>
     <col min="21" max="21" width="16"/>
-    <col min="22" max="26" width="12.7109375"/>
-    <col min="27" max="27" width="11.140625" customWidth="1"/>
-    <col min="28" max="32" width="12.7109375"/>
-    <col min="33" max="33" width="12.7109375" customWidth="1"/>
-    <col min="34" max="35" width="11.7109375" customWidth="1"/>
-    <col min="36" max="36" width="13.140625" customWidth="1"/>
-    <col min="37" max="37" width="11.85546875" customWidth="1"/>
-    <col min="42" max="45" width="12.7109375"/>
-    <col min="48" max="48" width="9" customWidth="1"/>
-    <col min="49" max="1035" width="8.5703125"/>
+    <col min="22" max="23" width="12.7109375"/>
+    <col min="24" max="24" width="10.85546875" customWidth="1"/>
+    <col min="25" max="27" width="12.7109375"/>
+    <col min="28" max="28" width="11.140625" customWidth="1"/>
+    <col min="29" max="33" width="12.7109375"/>
+    <col min="34" max="34" width="12.7109375" customWidth="1"/>
+    <col min="35" max="36" width="11.7109375" customWidth="1"/>
+    <col min="37" max="37" width="13.140625" customWidth="1"/>
+    <col min="38" max="38" width="11.85546875" customWidth="1"/>
+    <col min="43" max="46" width="12.7109375"/>
+    <col min="49" max="49" width="9" customWidth="1"/>
+    <col min="50" max="1036" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="AP1" s="1" t="s">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AQ1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AQ1" s="1"/>
       <c r="AR1" s="1"/>
       <c r="AS1" s="1"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
-    </row>
-    <row r="2" spans="1:48" s="4" customFormat="1" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AW1" s="1"/>
+    </row>
+    <row r="2" spans="1:49" s="4" customFormat="1" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
@@ -1454,45 +1468,45 @@
       <c r="W2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="Y2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Z2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="AA2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AH2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AH2" s="6" t="s">
+      <c r="AI2" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="AI2" s="6"/>
-      <c r="AJ2" s="4" t="s">
+      <c r="AJ2" s="6"/>
+      <c r="AK2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AK2" s="6"/>
       <c r="AL2" s="6"/>
-      <c r="AN2" s="6"/>
-      <c r="AO2" s="4" t="s">
+      <c r="AM2" s="6"/>
+      <c r="AO2" s="6"/>
+      <c r="AP2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AQ2" s="4" t="s">
+      <c r="AR2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AR2" s="4" t="s">
+      <c r="AS2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AU2" s="4" t="s">
+      <c r="AV2" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="AV2" s="4" t="s">
+      <c r="AW2" s="4" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:48" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:49" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>43</v>
       </c>
@@ -1518,109 +1532,110 @@
         <v>50</v>
       </c>
       <c r="T3" s="4"/>
-      <c r="AG3" s="4" t="s">
+      <c r="AH3" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AH3" s="4" t="s">
+      <c r="AI3" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="AI3" s="4"/>
-      <c r="AL3" s="4" t="s">
+      <c r="AJ3" s="4"/>
+      <c r="AM3" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="AM3" s="4" t="s">
+      <c r="AN3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AN3" s="4" t="s">
+      <c r="AO3" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AO3" s="4" t="s">
+      <c r="AP3" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AQ3" s="4" t="s">
+      <c r="AR3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AR3" s="4" t="s">
+      <c r="AS3" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:48" s="8" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+    <row r="4" spans="1:49" s="8" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="36" t="s">
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="36"/>
+      <c r="E4" s="32"/>
       <c r="F4" s="28"/>
       <c r="G4" s="28"/>
-      <c r="H4" s="37" t="s">
+      <c r="H4" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="I4" s="37"/>
+      <c r="I4" s="33"/>
       <c r="J4" s="29"/>
-      <c r="K4" s="32" t="s">
+      <c r="K4" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="L4" s="32"/>
+      <c r="L4" s="34"/>
       <c r="M4" s="30"/>
-      <c r="N4" s="33" t="s">
+      <c r="N4" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="O4" s="33"/>
-      <c r="P4" s="32" t="s">
+      <c r="O4" s="35"/>
+      <c r="P4" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="32"/>
-      <c r="S4" s="32"/>
-      <c r="T4" s="32"/>
-      <c r="U4" s="32"/>
-      <c r="V4" s="32"/>
-      <c r="W4" s="32"/>
-      <c r="X4" s="33" t="s">
+      <c r="Q4" s="34"/>
+      <c r="R4" s="34"/>
+      <c r="S4" s="34"/>
+      <c r="T4" s="34"/>
+      <c r="U4" s="34"/>
+      <c r="V4" s="34"/>
+      <c r="W4" s="34"/>
+      <c r="X4" s="38"/>
+      <c r="Y4" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="Y4" s="33"/>
-      <c r="Z4" s="33"/>
-      <c r="AA4" s="31" t="s">
+      <c r="Z4" s="35"/>
+      <c r="AA4" s="35"/>
+      <c r="AB4" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="AB4" s="31"/>
-      <c r="AC4" s="31"/>
-      <c r="AD4" s="7" t="s">
+      <c r="AC4" s="36"/>
+      <c r="AD4" s="36"/>
+      <c r="AE4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AE4" s="34" t="s">
+      <c r="AF4" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="AF4" s="34"/>
-      <c r="AG4" s="34"/>
-      <c r="AH4" s="31" t="s">
+      <c r="AG4" s="31"/>
+      <c r="AH4" s="31"/>
+      <c r="AI4" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="AI4" s="31"/>
-      <c r="AJ4" s="31"/>
-      <c r="AK4" s="22" t="s">
+      <c r="AJ4" s="36"/>
+      <c r="AK4" s="36"/>
+      <c r="AL4" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="AL4" s="22"/>
       <c r="AM4" s="22"/>
       <c r="AN4" s="22"/>
       <c r="AO4" s="22"/>
-      <c r="AP4" s="35" t="s">
+      <c r="AP4" s="22"/>
+      <c r="AQ4" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="AQ4" s="35"/>
-      <c r="AR4" s="35"/>
-      <c r="AS4" s="35"/>
-      <c r="AT4" s="16"/>
-      <c r="AU4" s="23"/>
-      <c r="AV4" s="21"/>
-    </row>
-    <row r="5" spans="1:48" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="AR4" s="37"/>
+      <c r="AS4" s="37"/>
+      <c r="AT4" s="37"/>
+      <c r="AU4" s="16"/>
+      <c r="AV4" s="23"/>
+      <c r="AW4" s="21"/>
+    </row>
+    <row r="5" spans="1:49" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>71</v>
       </c>
@@ -1691,82 +1706,85 @@
         <v>88</v>
       </c>
       <c r="X5" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="Y5" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="Y5" s="9" t="s">
+      <c r="Z5" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="Z5" s="9" t="s">
+      <c r="AA5" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="AA5" s="9" t="s">
+      <c r="AB5" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="AB5" s="9" t="s">
+      <c r="AC5" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="AC5" s="9" t="s">
+      <c r="AD5" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="AD5" s="9" t="s">
+      <c r="AE5" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="AE5" s="9" t="s">
+      <c r="AF5" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="AF5" s="9" t="s">
+      <c r="AG5" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="AG5" s="9" t="s">
+      <c r="AH5" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="AH5" s="9" t="s">
+      <c r="AI5" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="AI5" s="9" t="s">
+      <c r="AJ5" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="AJ5" s="9" t="s">
+      <c r="AK5" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AK5" s="9" t="s">
+      <c r="AL5" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="AL5" s="9" t="s">
+      <c r="AM5" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="AM5" s="9" t="s">
+      <c r="AN5" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="AN5" s="9" t="s">
+      <c r="AO5" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="AO5" s="9" t="s">
+      <c r="AP5" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="AP5" s="9" t="s">
+      <c r="AQ5" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="AQ5" s="9" t="s">
+      <c r="AR5" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="AR5" s="9" t="s">
+      <c r="AS5" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="AS5" s="9" t="s">
+      <c r="AT5" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="AT5" s="9" t="s">
+      <c r="AU5" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="AU5" s="9" t="s">
+      <c r="AV5" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="AV5" s="9" t="s">
+      <c r="AW5" s="9" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>170</v>
       </c>
@@ -1836,83 +1854,86 @@
       <c r="W6">
         <v>10</v>
       </c>
-      <c r="X6" s="12">
+      <c r="X6" s="27">
+        <v>0.04</v>
+      </c>
+      <c r="Y6" s="12">
         <v>0.03</v>
       </c>
-      <c r="Y6" s="12">
+      <c r="Z6" s="12">
         <v>0.01</v>
       </c>
-      <c r="Z6" s="12">
+      <c r="AA6" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AA6" s="12" t="s">
+      <c r="AB6" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="AB6" s="12">
+      <c r="AC6" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AC6" s="12">
-        <v>0</v>
-      </c>
-      <c r="AD6" t="s">
+      <c r="AD6" s="12">
+        <v>0</v>
+      </c>
+      <c r="AE6" t="s">
         <v>112</v>
       </c>
-      <c r="AE6" s="2" t="s">
+      <c r="AF6" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="AF6" s="2" t="s">
+      <c r="AG6" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="AG6">
+      <c r="AH6">
         <v>1</v>
       </c>
-      <c r="AH6" s="2" t="s">
+      <c r="AI6" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="AI6" s="18">
+      <c r="AJ6" s="18">
         <v>1</v>
       </c>
-      <c r="AJ6">
+      <c r="AK6">
         <v>200</v>
       </c>
-      <c r="AK6" t="s">
+      <c r="AL6" t="s">
         <v>142</v>
       </c>
-      <c r="AL6">
+      <c r="AM6">
         <v>5</v>
       </c>
-      <c r="AM6">
+      <c r="AN6">
         <v>200</v>
       </c>
-      <c r="AN6" s="2" t="s">
+      <c r="AO6" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="AO6">
+      <c r="AP6">
         <v>1</v>
       </c>
-      <c r="AP6" s="2" t="s">
+      <c r="AQ6" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AQ6" s="13">
+      <c r="AR6" s="13">
         <v>0.25</v>
       </c>
-      <c r="AR6" s="13">
+      <c r="AS6" s="13">
         <v>0.14499999999999999</v>
       </c>
-      <c r="AS6" s="13">
+      <c r="AT6" s="13">
         <v>0.05</v>
       </c>
-      <c r="AT6" s="19" t="b">
-        <v>0</v>
-      </c>
       <c r="AU6" s="19" t="b">
         <v>0</v>
       </c>
       <c r="AV6" s="19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AW6" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>181</v>
       </c>
@@ -1970,83 +1991,83 @@
       <c r="W9">
         <v>0</v>
       </c>
-      <c r="X9" s="27">
+      <c r="Y9" s="27">
         <v>0.03</v>
       </c>
-      <c r="Y9" s="27">
+      <c r="Z9" s="27">
         <v>0.01</v>
       </c>
-      <c r="Z9" s="27">
+      <c r="AA9" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AA9" s="27" t="s">
+      <c r="AB9" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="AB9" s="27">
+      <c r="AC9" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AC9" s="27">
-        <v>0</v>
-      </c>
-      <c r="AD9" t="s">
+      <c r="AD9" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE9" t="s">
         <v>112</v>
       </c>
-      <c r="AE9" s="2" t="s">
+      <c r="AF9" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="AF9" s="2" t="s">
+      <c r="AG9" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="AG9">
+      <c r="AH9">
         <v>1</v>
       </c>
-      <c r="AH9" s="2" t="s">
+      <c r="AI9" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="AI9" s="18">
+      <c r="AJ9" s="18">
         <v>1</v>
       </c>
-      <c r="AJ9">
+      <c r="AK9">
         <v>200</v>
       </c>
-      <c r="AK9" t="s">
+      <c r="AL9" t="s">
         <v>142</v>
       </c>
-      <c r="AL9">
+      <c r="AM9">
         <v>5</v>
       </c>
-      <c r="AM9">
+      <c r="AN9">
         <v>200</v>
       </c>
-      <c r="AN9" s="2" t="s">
+      <c r="AO9" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="AO9">
+      <c r="AP9">
         <v>1</v>
       </c>
-      <c r="AP9" s="2" t="s">
+      <c r="AQ9" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AQ9" s="13">
+      <c r="AR9" s="13">
         <v>0.25</v>
       </c>
-      <c r="AR9" s="13">
+      <c r="AS9" s="13">
         <v>0.14499999999999999</v>
       </c>
-      <c r="AS9" s="13">
+      <c r="AT9" s="13">
         <v>0.05</v>
       </c>
-      <c r="AT9" s="19" t="b">
-        <v>0</v>
-      </c>
       <c r="AU9" s="19" t="b">
         <v>0</v>
       </c>
       <c r="AV9" s="19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AW9" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>182</v>
       </c>
@@ -2104,83 +2125,83 @@
       <c r="W10">
         <v>0</v>
       </c>
-      <c r="X10" s="27">
+      <c r="Y10" s="27">
         <v>0.03</v>
       </c>
-      <c r="Y10" s="27">
+      <c r="Z10" s="27">
         <v>0.01</v>
       </c>
-      <c r="Z10" s="27">
+      <c r="AA10" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AA10" s="27" t="s">
+      <c r="AB10" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="AB10" s="27">
+      <c r="AC10" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AC10" s="27">
-        <v>0</v>
-      </c>
-      <c r="AD10" t="s">
+      <c r="AD10" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE10" t="s">
         <v>112</v>
       </c>
-      <c r="AE10" s="2" t="s">
+      <c r="AF10" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="AF10" s="2" t="s">
+      <c r="AG10" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="AG10">
+      <c r="AH10">
         <v>1</v>
       </c>
-      <c r="AH10" s="2" t="s">
+      <c r="AI10" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="AI10" s="18">
+      <c r="AJ10" s="18">
         <v>1</v>
       </c>
-      <c r="AJ10">
+      <c r="AK10">
         <v>200</v>
       </c>
-      <c r="AK10" t="s">
+      <c r="AL10" t="s">
         <v>142</v>
       </c>
-      <c r="AL10">
+      <c r="AM10">
         <v>5</v>
       </c>
-      <c r="AM10">
+      <c r="AN10">
         <v>200</v>
       </c>
-      <c r="AN10" s="2" t="s">
+      <c r="AO10" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="AO10">
+      <c r="AP10">
         <v>1</v>
       </c>
-      <c r="AP10" s="2" t="s">
+      <c r="AQ10" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AQ10" s="13">
+      <c r="AR10" s="13">
         <v>0.25</v>
       </c>
-      <c r="AR10" s="13">
+      <c r="AS10" s="13">
         <v>0.14499999999999999</v>
       </c>
-      <c r="AS10" s="13">
+      <c r="AT10" s="13">
         <v>0.05</v>
       </c>
-      <c r="AT10" s="19" t="b">
-        <v>0</v>
-      </c>
       <c r="AU10" s="19" t="b">
         <v>0</v>
       </c>
       <c r="AV10" s="19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AW10" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>183</v>
       </c>
@@ -2238,87 +2259,87 @@
       <c r="W11">
         <v>0</v>
       </c>
-      <c r="X11" s="27">
+      <c r="Y11" s="27">
         <v>0.03</v>
       </c>
-      <c r="Y11" s="27">
+      <c r="Z11" s="27">
         <v>0.01</v>
       </c>
-      <c r="Z11" s="27">
+      <c r="AA11" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AA11" s="27" t="s">
+      <c r="AB11" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="AB11" s="27">
+      <c r="AC11" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AC11" s="27">
-        <v>0</v>
-      </c>
-      <c r="AD11" t="s">
+      <c r="AD11" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE11" t="s">
         <v>112</v>
       </c>
-      <c r="AE11" s="2" t="s">
+      <c r="AF11" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="AF11" s="2" t="s">
+      <c r="AG11" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="AG11">
+      <c r="AH11">
         <v>1</v>
       </c>
-      <c r="AH11" s="2" t="s">
+      <c r="AI11" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="AI11" s="18">
+      <c r="AJ11" s="18">
         <v>1</v>
       </c>
-      <c r="AJ11">
+      <c r="AK11">
         <v>200</v>
       </c>
-      <c r="AK11" t="s">
+      <c r="AL11" t="s">
         <v>142</v>
       </c>
-      <c r="AL11">
+      <c r="AM11">
         <v>5</v>
       </c>
-      <c r="AM11">
+      <c r="AN11">
         <v>200</v>
       </c>
-      <c r="AN11" s="2" t="s">
+      <c r="AO11" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="AO11">
+      <c r="AP11">
         <v>1</v>
       </c>
-      <c r="AP11" s="2" t="s">
+      <c r="AQ11" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AQ11" s="13">
+      <c r="AR11" s="13">
         <v>0.25</v>
       </c>
-      <c r="AR11" s="13">
+      <c r="AS11" s="13">
         <v>0.14499999999999999</v>
       </c>
-      <c r="AS11" s="13">
+      <c r="AT11" s="13">
         <v>0.05</v>
       </c>
-      <c r="AT11" s="19" t="b">
-        <v>0</v>
-      </c>
       <c r="AU11" s="19" t="b">
         <v>0</v>
       </c>
       <c r="AV11" s="19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AW11" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
       <c r="C12" s="27"/>
       <c r="D12" s="27"/>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>184</v>
       </c>
@@ -2376,83 +2397,83 @@
       <c r="W13">
         <v>0</v>
       </c>
-      <c r="X13" s="27">
+      <c r="Y13" s="27">
         <v>0.03</v>
       </c>
-      <c r="Y13" s="27">
+      <c r="Z13" s="27">
         <v>0.01</v>
       </c>
-      <c r="Z13" s="27">
+      <c r="AA13" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AA13" s="27" t="s">
+      <c r="AB13" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="AB13" s="27">
+      <c r="AC13" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AC13" s="27">
-        <v>0</v>
-      </c>
-      <c r="AD13" t="s">
+      <c r="AD13" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE13" t="s">
         <v>112</v>
       </c>
-      <c r="AE13" s="2" t="s">
+      <c r="AF13" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="AF13" s="2" t="s">
+      <c r="AG13" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="AG13">
+      <c r="AH13">
         <v>1</v>
       </c>
-      <c r="AH13" s="2" t="s">
+      <c r="AI13" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="AI13" s="18">
+      <c r="AJ13" s="18">
         <v>1</v>
       </c>
-      <c r="AJ13">
+      <c r="AK13">
         <v>200</v>
       </c>
-      <c r="AK13" t="s">
+      <c r="AL13" t="s">
         <v>142</v>
       </c>
-      <c r="AL13">
+      <c r="AM13">
         <v>5</v>
       </c>
-      <c r="AM13">
+      <c r="AN13">
         <v>200</v>
       </c>
-      <c r="AN13" s="2" t="s">
+      <c r="AO13" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="AO13">
+      <c r="AP13">
         <v>1</v>
       </c>
-      <c r="AP13" s="2" t="s">
+      <c r="AQ13" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AQ13" s="13">
+      <c r="AR13" s="13">
         <v>0.25</v>
       </c>
-      <c r="AR13" s="13">
+      <c r="AS13" s="13">
         <v>0.14499999999999999</v>
       </c>
-      <c r="AS13" s="13">
+      <c r="AT13" s="13">
         <v>0.05</v>
       </c>
-      <c r="AT13" s="19" t="b">
-        <v>0</v>
-      </c>
       <c r="AU13" s="19" t="b">
         <v>0</v>
       </c>
       <c r="AV13" s="19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AW13" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>185</v>
       </c>
@@ -2510,83 +2531,83 @@
       <c r="W14">
         <v>0</v>
       </c>
-      <c r="X14" s="27">
+      <c r="Y14" s="27">
         <v>0.03</v>
       </c>
-      <c r="Y14" s="27">
+      <c r="Z14" s="27">
         <v>0.01</v>
       </c>
-      <c r="Z14" s="27">
+      <c r="AA14" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AA14" s="27" t="s">
+      <c r="AB14" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="AB14" s="27">
+      <c r="AC14" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AC14" s="27">
-        <v>0</v>
-      </c>
-      <c r="AD14" t="s">
+      <c r="AD14" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE14" t="s">
         <v>112</v>
       </c>
-      <c r="AE14" s="2" t="s">
+      <c r="AF14" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="AF14" s="2" t="s">
+      <c r="AG14" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="AG14">
+      <c r="AH14">
         <v>1</v>
       </c>
-      <c r="AH14" s="2" t="s">
+      <c r="AI14" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="AI14" s="18">
+      <c r="AJ14" s="18">
         <v>1</v>
       </c>
-      <c r="AJ14">
+      <c r="AK14">
         <v>200</v>
       </c>
-      <c r="AK14" t="s">
+      <c r="AL14" t="s">
         <v>142</v>
       </c>
-      <c r="AL14">
+      <c r="AM14">
         <v>5</v>
       </c>
-      <c r="AM14">
+      <c r="AN14">
         <v>200</v>
       </c>
-      <c r="AN14" s="2" t="s">
+      <c r="AO14" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="AO14">
+      <c r="AP14">
         <v>1</v>
       </c>
-      <c r="AP14" s="2" t="s">
+      <c r="AQ14" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AQ14" s="13">
+      <c r="AR14" s="13">
         <v>0.25</v>
       </c>
-      <c r="AR14" s="13">
+      <c r="AS14" s="13">
         <v>0.14499999999999999</v>
       </c>
-      <c r="AS14" s="13">
+      <c r="AT14" s="13">
         <v>0.05</v>
       </c>
-      <c r="AT14" s="19" t="b">
-        <v>0</v>
-      </c>
       <c r="AU14" s="19" t="b">
         <v>0</v>
       </c>
       <c r="AV14" s="19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AW14" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>186</v>
       </c>
@@ -2644,86 +2665,86 @@
       <c r="W15">
         <v>0</v>
       </c>
-      <c r="X15" s="27">
+      <c r="Y15" s="27">
         <v>0.03</v>
       </c>
-      <c r="Y15" s="27">
+      <c r="Z15" s="27">
         <v>0.01</v>
       </c>
-      <c r="Z15" s="27">
+      <c r="AA15" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AA15" s="27" t="s">
+      <c r="AB15" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="AB15" s="27">
+      <c r="AC15" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AC15" s="27">
-        <v>0</v>
-      </c>
-      <c r="AD15" t="s">
+      <c r="AD15" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE15" t="s">
         <v>112</v>
       </c>
-      <c r="AE15" s="2" t="s">
+      <c r="AF15" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="AF15" s="2" t="s">
+      <c r="AG15" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="AG15">
+      <c r="AH15">
         <v>1</v>
       </c>
-      <c r="AH15" s="2" t="s">
+      <c r="AI15" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="AI15" s="18">
+      <c r="AJ15" s="18">
         <v>1</v>
       </c>
-      <c r="AJ15">
+      <c r="AK15">
         <v>200</v>
       </c>
-      <c r="AK15" t="s">
+      <c r="AL15" t="s">
         <v>142</v>
       </c>
-      <c r="AL15">
+      <c r="AM15">
         <v>5</v>
       </c>
-      <c r="AM15">
+      <c r="AN15">
         <v>200</v>
       </c>
-      <c r="AN15" s="2" t="s">
+      <c r="AO15" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="AO15">
+      <c r="AP15">
         <v>1</v>
       </c>
-      <c r="AP15" s="2" t="s">
+      <c r="AQ15" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AQ15" s="13">
+      <c r="AR15" s="13">
         <v>0.25</v>
       </c>
-      <c r="AR15" s="13">
+      <c r="AS15" s="13">
         <v>0.14499999999999999</v>
       </c>
-      <c r="AS15" s="13">
+      <c r="AT15" s="13">
         <v>0.05</v>
       </c>
-      <c r="AT15" s="19" t="b">
-        <v>0</v>
-      </c>
       <c r="AU15" s="19" t="b">
         <v>0</v>
       </c>
       <c r="AV15" s="19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AW15" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
       <c r="C16" s="11"/>
     </row>
-    <row r="17" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>187</v>
       </c>
@@ -2781,83 +2802,83 @@
       <c r="W17">
         <v>0</v>
       </c>
-      <c r="X17" s="27">
+      <c r="Y17" s="27">
         <v>0.03</v>
       </c>
-      <c r="Y17" s="27">
+      <c r="Z17" s="27">
         <v>0.01</v>
       </c>
-      <c r="Z17" s="27">
+      <c r="AA17" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AA17" s="27" t="s">
+      <c r="AB17" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="AB17" s="27">
+      <c r="AC17" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AC17" s="27">
-        <v>0</v>
-      </c>
-      <c r="AD17" t="s">
+      <c r="AD17" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE17" t="s">
         <v>112</v>
       </c>
-      <c r="AE17" s="2" t="s">
+      <c r="AF17" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="AF17" s="2" t="s">
+      <c r="AG17" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="AG17">
+      <c r="AH17">
         <v>1</v>
       </c>
-      <c r="AH17" s="2" t="s">
+      <c r="AI17" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="AI17" s="18">
+      <c r="AJ17" s="18">
         <v>1</v>
       </c>
-      <c r="AJ17">
+      <c r="AK17">
         <v>200</v>
       </c>
-      <c r="AK17" t="s">
+      <c r="AL17" t="s">
         <v>142</v>
       </c>
-      <c r="AL17">
+      <c r="AM17">
         <v>5</v>
       </c>
-      <c r="AM17">
+      <c r="AN17">
         <v>200</v>
       </c>
-      <c r="AN17" s="2" t="s">
+      <c r="AO17" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="AO17">
+      <c r="AP17">
         <v>1</v>
       </c>
-      <c r="AP17" s="2" t="s">
+      <c r="AQ17" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AQ17" s="13">
+      <c r="AR17" s="13">
         <v>0.25</v>
       </c>
-      <c r="AR17" s="13">
+      <c r="AS17" s="13">
         <v>0.14499999999999999</v>
       </c>
-      <c r="AS17" s="13">
+      <c r="AT17" s="13">
         <v>0.05</v>
       </c>
-      <c r="AT17" s="19" t="b">
-        <v>0</v>
-      </c>
       <c r="AU17" s="19" t="b">
         <v>0</v>
       </c>
       <c r="AV17" s="19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AW17" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>188</v>
       </c>
@@ -2915,83 +2936,83 @@
       <c r="W18">
         <v>0</v>
       </c>
-      <c r="X18" s="27">
+      <c r="Y18" s="27">
         <v>0.03</v>
       </c>
-      <c r="Y18" s="27">
+      <c r="Z18" s="27">
         <v>0.01</v>
       </c>
-      <c r="Z18" s="27">
+      <c r="AA18" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AA18" s="27" t="s">
+      <c r="AB18" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="AB18" s="27">
+      <c r="AC18" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AC18" s="27">
-        <v>0</v>
-      </c>
-      <c r="AD18" t="s">
+      <c r="AD18" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE18" t="s">
         <v>112</v>
       </c>
-      <c r="AE18" s="2" t="s">
+      <c r="AF18" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="AF18" s="2" t="s">
+      <c r="AG18" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="AG18">
+      <c r="AH18">
         <v>1</v>
       </c>
-      <c r="AH18" s="2" t="s">
+      <c r="AI18" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="AI18" s="18">
+      <c r="AJ18" s="18">
         <v>1</v>
       </c>
-      <c r="AJ18">
+      <c r="AK18">
         <v>200</v>
       </c>
-      <c r="AK18" t="s">
+      <c r="AL18" t="s">
         <v>142</v>
       </c>
-      <c r="AL18">
+      <c r="AM18">
         <v>5</v>
       </c>
-      <c r="AM18">
+      <c r="AN18">
         <v>200</v>
       </c>
-      <c r="AN18" s="2" t="s">
+      <c r="AO18" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="AO18">
+      <c r="AP18">
         <v>1</v>
       </c>
-      <c r="AP18" s="2" t="s">
+      <c r="AQ18" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AQ18" s="13">
+      <c r="AR18" s="13">
         <v>0.25</v>
       </c>
-      <c r="AR18" s="13">
+      <c r="AS18" s="13">
         <v>0.14499999999999999</v>
       </c>
-      <c r="AS18" s="13">
+      <c r="AT18" s="13">
         <v>0.05</v>
       </c>
-      <c r="AT18" s="19" t="b">
-        <v>0</v>
-      </c>
       <c r="AU18" s="19" t="b">
         <v>0</v>
       </c>
       <c r="AV18" s="19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AW18" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>189</v>
       </c>
@@ -3049,110 +3070,110 @@
       <c r="W19">
         <v>0</v>
       </c>
-      <c r="X19" s="27">
+      <c r="Y19" s="27">
         <v>0.03</v>
       </c>
-      <c r="Y19" s="27">
+      <c r="Z19" s="27">
         <v>0.01</v>
       </c>
-      <c r="Z19" s="27">
+      <c r="AA19" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AA19" s="27" t="s">
+      <c r="AB19" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="AB19" s="27">
+      <c r="AC19" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AC19" s="27">
-        <v>0</v>
-      </c>
-      <c r="AD19" t="s">
+      <c r="AD19" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE19" t="s">
         <v>112</v>
       </c>
-      <c r="AE19" s="2" t="s">
+      <c r="AF19" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="AF19" s="2" t="s">
+      <c r="AG19" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="AG19">
+      <c r="AH19">
         <v>1</v>
       </c>
-      <c r="AH19" s="2" t="s">
+      <c r="AI19" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="AI19" s="18">
+      <c r="AJ19" s="18">
         <v>1</v>
       </c>
-      <c r="AJ19">
+      <c r="AK19">
         <v>200</v>
       </c>
-      <c r="AK19" t="s">
+      <c r="AL19" t="s">
         <v>142</v>
       </c>
-      <c r="AL19">
+      <c r="AM19">
         <v>5</v>
       </c>
-      <c r="AM19">
+      <c r="AN19">
         <v>200</v>
       </c>
-      <c r="AN19" s="2" t="s">
+      <c r="AO19" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="AO19">
+      <c r="AP19">
         <v>1</v>
       </c>
-      <c r="AP19" s="2" t="s">
+      <c r="AQ19" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AQ19" s="13">
+      <c r="AR19" s="13">
         <v>0.25</v>
       </c>
-      <c r="AR19" s="13">
+      <c r="AS19" s="13">
         <v>0.14499999999999999</v>
       </c>
-      <c r="AS19" s="13">
+      <c r="AT19" s="13">
         <v>0.05</v>
       </c>
-      <c r="AT19" s="19" t="b">
-        <v>0</v>
-      </c>
       <c r="AU19" s="19" t="b">
         <v>0</v>
       </c>
       <c r="AV19" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AW19" s="19" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="AI4:AK4"/>
+    <mergeCell ref="P4:W4"/>
+    <mergeCell ref="Y4:AA4"/>
+    <mergeCell ref="AF4:AH4"/>
+    <mergeCell ref="AQ4:AT4"/>
+    <mergeCell ref="AB4:AD4"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="N4:O4"/>
-    <mergeCell ref="AH4:AJ4"/>
-    <mergeCell ref="P4:W4"/>
-    <mergeCell ref="X4:Z4"/>
-    <mergeCell ref="AE4:AG4"/>
-    <mergeCell ref="AP4:AS4"/>
-    <mergeCell ref="AA4:AC4"/>
   </mergeCells>
   <dataValidations count="23">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN6 AN9:AN11 AN13:AN15 AN17:AN19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO6 AO9:AO11 AO13:AO15 AO17:AO19">
       <formula1>"MA,EAA"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF6 AF9:AF11 AF13:AF15 AF17:AF19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG6 AG9:AG11 AG13:AG15 AG17:AG19">
       <formula1>"cd,cp,sl"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE6 AE9:AE11 AE13:AE15 AE17:AE19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF6 AF9:AF11 AF13:AF15 AF17:AF19">
       <formula1>"open,closed"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP6 AP9:AP11 AP13:AP15 AP17:AP19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ6 AQ9:AQ11 AQ13:AQ15 AQ17:AQ19">
       <formula1>ConPolicy</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3164,54 +3185,54 @@
       <formula1>55</formula1>
       <formula2>65</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="U6 Y6 U9:U11 Y9:Y11 U13:U15 Y13:Y15 U17:U19 Y17:Y19">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="U6 Z6 U9:U11 Z9:Z11 U13:U15 Z13:Z15 U17:U19 Z17:Z19">
       <formula1>0</formula1>
       <formula2>0.1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="V6:W6 V13:V15 V17:V19 V9:V11 W9:W19">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="W9:X19 V13:V15 V17:V19 V9:V11 V6:W6">
       <formula1>0</formula1>
       <formula2>15</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="X6 AB6 Z6 X9:X11 AB9:AB11 Z9:Z11 X13:X15 AB13:AB15 Z13:Z15 X17:X19 AB17:AB19 Z17:Z19">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="X6:Y6 AC6 AA6 Y9:Y11 AC9:AC11 AA9:AA11 Y13:Y15 AC13:AC15 AA13:AA15 Y17:Y19 AC17:AC19 AA17:AA19">
       <formula1>0</formula1>
       <formula2>0.2</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AG6 AG9:AG11 AG13:AG15 AG17:AG19">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AH6 AH9:AH11 AH13:AH15 AH17:AH19">
       <formula1>0</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AQ6:AR6 AQ9:AR11 AQ13:AR15 AQ17:AR19">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AR6:AS6 AR9:AS11 AR13:AS15 AR17:AS19">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AS6 AS9:AS11 AS13:AS15 AS17:AS19">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AT6 AT9:AT11 AT13:AT15 AT17:AT19">
       <formula1>0</formula1>
       <formula2>0.3</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="AC6 AC9:AC11 AC13:AC15 AC17:AC19">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="AD6 AD9:AD11 AD13:AD15 AD17:AD19">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AL6 AL9:AL11 AL13:AL15 AL17:AL19">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AM6 AM9:AM11 AM13:AM15 AM17:AM19">
       <formula1>1</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM6 AM9:AM11 AM13:AM15 AM17:AM19">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN6 AN9:AN11 AN13:AN15 AN17:AN19">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO6 AO9:AO11 AO13:AO15 AO17:AO19">
+    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP6 AP9:AP11 AP13:AP15 AP17:AP19">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="AA6 AA9:AA11 AA13:AA15 AA17:AA19"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AT6:AV6 AT9:AV11 AT13:AV15 AT17:AV19">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="AB6 AB9:AB11 AB13:AB15 AB17:AB19"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AU6:AW6 AU9:AW11 AU13:AW15 AU17:AW19">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH6 AH9:AH11 AH13:AH15 AH17:AH19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI6 AI9:AI11 AI13:AI15 AI17:AI19">
       <formula1>"MA,AL,AL_pct"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI6 AI9:AI11 AI13:AI15 AI17:AI19">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ6 AJ9:AJ11 AJ13:AJ15 AJ17:AJ19">
       <formula1>0</formula1>
       <formula2>1.5</formula2>
     </dataValidation>
@@ -3433,8 +3454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3472,7 +3493,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="B3">
         <v>10</v>

</xml_diff>

<commit_message>
new parameters for salary growth assumptions
</commit_message>
<xml_diff>
--- a/IO_Dev/RunControl_Dev.xlsx
+++ b/IO_Dev/RunControl_Dev.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="7230" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="7230" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="203">
   <si>
     <t>Sheet #</t>
   </si>
@@ -635,7 +635,10 @@
     <t>n_init_actives</t>
   </si>
   <si>
-    <t>startingSal.growth</t>
+    <t>startingSal_growth</t>
+  </si>
+  <si>
+    <t>salgrowth_amort</t>
   </si>
 </sst>
 </file>
@@ -1374,13 +1377,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW19"/>
+  <dimension ref="A1:AX19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="P6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="G26" sqref="G26"/>
+      <selection pane="bottomRight" activeCell="Y7" sqref="Y7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1397,31 +1400,31 @@
     <col min="16" max="20" width="9.28515625" customWidth="1"/>
     <col min="21" max="21" width="16"/>
     <col min="22" max="23" width="12.7109375"/>
-    <col min="24" max="24" width="10.85546875" customWidth="1"/>
-    <col min="25" max="27" width="12.7109375"/>
-    <col min="28" max="28" width="11.140625" customWidth="1"/>
-    <col min="29" max="33" width="12.7109375"/>
-    <col min="34" max="34" width="12.7109375" customWidth="1"/>
-    <col min="35" max="36" width="11.7109375" customWidth="1"/>
-    <col min="37" max="37" width="13.140625" customWidth="1"/>
-    <col min="38" max="38" width="11.85546875" customWidth="1"/>
-    <col min="43" max="46" width="12.7109375"/>
-    <col min="49" max="49" width="9" customWidth="1"/>
-    <col min="50" max="1036" width="8.5703125"/>
+    <col min="24" max="25" width="10.85546875" customWidth="1"/>
+    <col min="26" max="28" width="12.7109375"/>
+    <col min="29" max="29" width="11.140625" customWidth="1"/>
+    <col min="30" max="34" width="12.7109375"/>
+    <col min="35" max="35" width="12.7109375" customWidth="1"/>
+    <col min="36" max="37" width="11.7109375" customWidth="1"/>
+    <col min="38" max="38" width="13.140625" customWidth="1"/>
+    <col min="39" max="39" width="11.85546875" customWidth="1"/>
+    <col min="44" max="47" width="12.7109375"/>
+    <col min="50" max="50" width="9" customWidth="1"/>
+    <col min="51" max="1037" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="AQ1" s="1" t="s">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AR1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AR1" s="1"/>
       <c r="AS1" s="1"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
       <c r="AW1" s="1"/>
-    </row>
-    <row r="2" spans="1:49" s="4" customFormat="1" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AX1" s="1"/>
+    </row>
+    <row r="2" spans="1:50" s="4" customFormat="1" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
@@ -1468,45 +1471,45 @@
       <c r="W2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Z2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="AA2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AB2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AH2" s="4" t="s">
+      <c r="AI2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AI2" s="6" t="s">
+      <c r="AJ2" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="AJ2" s="6"/>
-      <c r="AK2" s="4" t="s">
+      <c r="AK2" s="6"/>
+      <c r="AL2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AL2" s="6"/>
       <c r="AM2" s="6"/>
-      <c r="AO2" s="6"/>
-      <c r="AP2" s="4" t="s">
+      <c r="AN2" s="6"/>
+      <c r="AP2" s="6"/>
+      <c r="AQ2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AR2" s="4" t="s">
+      <c r="AS2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AS2" s="4" t="s">
+      <c r="AT2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AV2" s="4" t="s">
+      <c r="AW2" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="AW2" s="4" t="s">
+      <c r="AX2" s="4" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:49" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>43</v>
       </c>
@@ -1532,33 +1535,33 @@
         <v>50</v>
       </c>
       <c r="T3" s="4"/>
-      <c r="AH3" s="4" t="s">
+      <c r="AI3" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AI3" s="4" t="s">
+      <c r="AJ3" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="AJ3" s="4"/>
-      <c r="AM3" s="4" t="s">
+      <c r="AK3" s="4"/>
+      <c r="AN3" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="AN3" s="4" t="s">
+      <c r="AO3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AO3" s="4" t="s">
+      <c r="AP3" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AP3" s="4" t="s">
+      <c r="AQ3" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AR3" s="4" t="s">
+      <c r="AS3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AS3" s="4" t="s">
+      <c r="AT3" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:49" s="8" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:50" s="8" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>58</v>
       </c>
@@ -1595,47 +1598,48 @@
       <c r="V4" s="34"/>
       <c r="W4" s="34"/>
       <c r="X4" s="38"/>
-      <c r="Y4" s="35" t="s">
+      <c r="Y4" s="38"/>
+      <c r="Z4" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="Z4" s="35"/>
       <c r="AA4" s="35"/>
-      <c r="AB4" s="36" t="s">
+      <c r="AB4" s="35"/>
+      <c r="AC4" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="AC4" s="36"/>
       <c r="AD4" s="36"/>
-      <c r="AE4" s="7" t="s">
+      <c r="AE4" s="36"/>
+      <c r="AF4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AF4" s="31" t="s">
+      <c r="AG4" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="AG4" s="31"/>
       <c r="AH4" s="31"/>
-      <c r="AI4" s="36" t="s">
+      <c r="AI4" s="31"/>
+      <c r="AJ4" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="AJ4" s="36"/>
       <c r="AK4" s="36"/>
-      <c r="AL4" s="22" t="s">
+      <c r="AL4" s="36"/>
+      <c r="AM4" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="AM4" s="22"/>
       <c r="AN4" s="22"/>
       <c r="AO4" s="22"/>
       <c r="AP4" s="22"/>
-      <c r="AQ4" s="37" t="s">
+      <c r="AQ4" s="22"/>
+      <c r="AR4" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="AR4" s="37"/>
       <c r="AS4" s="37"/>
       <c r="AT4" s="37"/>
-      <c r="AU4" s="16"/>
-      <c r="AV4" s="23"/>
-      <c r="AW4" s="21"/>
-    </row>
-    <row r="5" spans="1:49" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="AU4" s="37"/>
+      <c r="AV4" s="16"/>
+      <c r="AW4" s="23"/>
+      <c r="AX4" s="21"/>
+    </row>
+    <row r="5" spans="1:50" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>71</v>
       </c>
@@ -1709,82 +1713,85 @@
         <v>201</v>
       </c>
       <c r="Y5" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="Z5" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="Z5" s="9" t="s">
+      <c r="AA5" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AA5" s="9" t="s">
+      <c r="AB5" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="AB5" s="9" t="s">
+      <c r="AC5" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="AC5" s="9" t="s">
+      <c r="AD5" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="AD5" s="9" t="s">
+      <c r="AE5" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="AE5" s="9" t="s">
+      <c r="AF5" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="AF5" s="9" t="s">
+      <c r="AG5" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="AG5" s="9" t="s">
+      <c r="AH5" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="AH5" s="9" t="s">
+      <c r="AI5" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="AI5" s="9" t="s">
+      <c r="AJ5" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="AJ5" s="9" t="s">
+      <c r="AK5" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="AK5" s="9" t="s">
+      <c r="AL5" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AL5" s="9" t="s">
+      <c r="AM5" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="AM5" s="9" t="s">
+      <c r="AN5" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="AN5" s="9" t="s">
+      <c r="AO5" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="AO5" s="9" t="s">
+      <c r="AP5" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="AP5" s="9" t="s">
+      <c r="AQ5" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="AQ5" s="9" t="s">
+      <c r="AR5" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="AR5" s="9" t="s">
+      <c r="AS5" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="AS5" s="9" t="s">
+      <c r="AT5" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="AT5" s="9" t="s">
+      <c r="AU5" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="AU5" s="9" t="s">
+      <c r="AV5" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="AV5" s="9" t="s">
+      <c r="AW5" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="AW5" s="9" t="s">
+      <c r="AX5" s="9" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>170</v>
       </c>
@@ -1857,83 +1864,86 @@
       <c r="X6" s="27">
         <v>0.04</v>
       </c>
-      <c r="Y6" s="12">
+      <c r="Y6" s="27">
+        <v>0.04</v>
+      </c>
+      <c r="Z6" s="12">
         <v>0.03</v>
       </c>
-      <c r="Z6" s="12">
+      <c r="AA6" s="12">
         <v>0.01</v>
       </c>
-      <c r="AA6" s="12">
+      <c r="AB6" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AB6" s="12" t="s">
+      <c r="AC6" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="AC6" s="12">
+      <c r="AD6" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AD6" s="12">
-        <v>0</v>
-      </c>
-      <c r="AE6" t="s">
+      <c r="AE6" s="12">
+        <v>0</v>
+      </c>
+      <c r="AF6" t="s">
         <v>112</v>
       </c>
-      <c r="AF6" s="2" t="s">
+      <c r="AG6" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="AG6" s="2" t="s">
+      <c r="AH6" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="AH6">
+      <c r="AI6">
         <v>1</v>
       </c>
-      <c r="AI6" s="2" t="s">
+      <c r="AJ6" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="AJ6" s="18">
+      <c r="AK6" s="18">
         <v>1</v>
       </c>
-      <c r="AK6">
+      <c r="AL6">
         <v>200</v>
       </c>
-      <c r="AL6" t="s">
+      <c r="AM6" t="s">
         <v>142</v>
       </c>
-      <c r="AM6">
+      <c r="AN6">
         <v>5</v>
       </c>
-      <c r="AN6">
+      <c r="AO6">
         <v>200</v>
       </c>
-      <c r="AO6" s="2" t="s">
+      <c r="AP6" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="AP6">
+      <c r="AQ6">
         <v>1</v>
       </c>
-      <c r="AQ6" s="2" t="s">
+      <c r="AR6" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AR6" s="13">
+      <c r="AS6" s="13">
         <v>0.25</v>
       </c>
-      <c r="AS6" s="13">
+      <c r="AT6" s="13">
         <v>0.14499999999999999</v>
       </c>
-      <c r="AT6" s="13">
+      <c r="AU6" s="13">
         <v>0.05</v>
       </c>
-      <c r="AU6" s="19" t="b">
-        <v>0</v>
-      </c>
       <c r="AV6" s="19" t="b">
         <v>0</v>
       </c>
       <c r="AW6" s="19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AX6" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>181</v>
       </c>
@@ -1991,83 +2001,83 @@
       <c r="W9">
         <v>0</v>
       </c>
-      <c r="Y9" s="27">
+      <c r="Z9" s="27">
         <v>0.03</v>
       </c>
-      <c r="Z9" s="27">
+      <c r="AA9" s="27">
         <v>0.01</v>
       </c>
-      <c r="AA9" s="27">
+      <c r="AB9" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AB9" s="27" t="s">
+      <c r="AC9" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="AC9" s="27">
+      <c r="AD9" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AD9" s="27">
-        <v>0</v>
-      </c>
-      <c r="AE9" t="s">
+      <c r="AE9" s="27">
+        <v>0</v>
+      </c>
+      <c r="AF9" t="s">
         <v>112</v>
       </c>
-      <c r="AF9" s="2" t="s">
+      <c r="AG9" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="AG9" s="2" t="s">
+      <c r="AH9" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="AH9">
+      <c r="AI9">
         <v>1</v>
       </c>
-      <c r="AI9" s="2" t="s">
+      <c r="AJ9" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="AJ9" s="18">
+      <c r="AK9" s="18">
         <v>1</v>
       </c>
-      <c r="AK9">
+      <c r="AL9">
         <v>200</v>
       </c>
-      <c r="AL9" t="s">
+      <c r="AM9" t="s">
         <v>142</v>
       </c>
-      <c r="AM9">
+      <c r="AN9">
         <v>5</v>
       </c>
-      <c r="AN9">
+      <c r="AO9">
         <v>200</v>
       </c>
-      <c r="AO9" s="2" t="s">
+      <c r="AP9" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="AP9">
+      <c r="AQ9">
         <v>1</v>
       </c>
-      <c r="AQ9" s="2" t="s">
+      <c r="AR9" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AR9" s="13">
+      <c r="AS9" s="13">
         <v>0.25</v>
       </c>
-      <c r="AS9" s="13">
+      <c r="AT9" s="13">
         <v>0.14499999999999999</v>
       </c>
-      <c r="AT9" s="13">
+      <c r="AU9" s="13">
         <v>0.05</v>
       </c>
-      <c r="AU9" s="19" t="b">
-        <v>0</v>
-      </c>
       <c r="AV9" s="19" t="b">
         <v>0</v>
       </c>
       <c r="AW9" s="19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AX9" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>182</v>
       </c>
@@ -2125,83 +2135,83 @@
       <c r="W10">
         <v>0</v>
       </c>
-      <c r="Y10" s="27">
+      <c r="Z10" s="27">
         <v>0.03</v>
       </c>
-      <c r="Z10" s="27">
+      <c r="AA10" s="27">
         <v>0.01</v>
       </c>
-      <c r="AA10" s="27">
+      <c r="AB10" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AB10" s="27" t="s">
+      <c r="AC10" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="AC10" s="27">
+      <c r="AD10" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AD10" s="27">
-        <v>0</v>
-      </c>
-      <c r="AE10" t="s">
+      <c r="AE10" s="27">
+        <v>0</v>
+      </c>
+      <c r="AF10" t="s">
         <v>112</v>
       </c>
-      <c r="AF10" s="2" t="s">
+      <c r="AG10" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="AG10" s="2" t="s">
+      <c r="AH10" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="AH10">
+      <c r="AI10">
         <v>1</v>
       </c>
-      <c r="AI10" s="2" t="s">
+      <c r="AJ10" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="AJ10" s="18">
+      <c r="AK10" s="18">
         <v>1</v>
       </c>
-      <c r="AK10">
+      <c r="AL10">
         <v>200</v>
       </c>
-      <c r="AL10" t="s">
+      <c r="AM10" t="s">
         <v>142</v>
       </c>
-      <c r="AM10">
+      <c r="AN10">
         <v>5</v>
       </c>
-      <c r="AN10">
+      <c r="AO10">
         <v>200</v>
       </c>
-      <c r="AO10" s="2" t="s">
+      <c r="AP10" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="AP10">
+      <c r="AQ10">
         <v>1</v>
       </c>
-      <c r="AQ10" s="2" t="s">
+      <c r="AR10" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AR10" s="13">
+      <c r="AS10" s="13">
         <v>0.25</v>
       </c>
-      <c r="AS10" s="13">
+      <c r="AT10" s="13">
         <v>0.14499999999999999</v>
       </c>
-      <c r="AT10" s="13">
+      <c r="AU10" s="13">
         <v>0.05</v>
       </c>
-      <c r="AU10" s="19" t="b">
-        <v>0</v>
-      </c>
       <c r="AV10" s="19" t="b">
         <v>0</v>
       </c>
       <c r="AW10" s="19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AX10" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>183</v>
       </c>
@@ -2259,87 +2269,87 @@
       <c r="W11">
         <v>0</v>
       </c>
-      <c r="Y11" s="27">
+      <c r="Z11" s="27">
         <v>0.03</v>
       </c>
-      <c r="Z11" s="27">
+      <c r="AA11" s="27">
         <v>0.01</v>
       </c>
-      <c r="AA11" s="27">
+      <c r="AB11" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AB11" s="27" t="s">
+      <c r="AC11" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="AC11" s="27">
+      <c r="AD11" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AD11" s="27">
-        <v>0</v>
-      </c>
-      <c r="AE11" t="s">
+      <c r="AE11" s="27">
+        <v>0</v>
+      </c>
+      <c r="AF11" t="s">
         <v>112</v>
       </c>
-      <c r="AF11" s="2" t="s">
+      <c r="AG11" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="AG11" s="2" t="s">
+      <c r="AH11" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="AH11">
+      <c r="AI11">
         <v>1</v>
       </c>
-      <c r="AI11" s="2" t="s">
+      <c r="AJ11" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="AJ11" s="18">
+      <c r="AK11" s="18">
         <v>1</v>
       </c>
-      <c r="AK11">
+      <c r="AL11">
         <v>200</v>
       </c>
-      <c r="AL11" t="s">
+      <c r="AM11" t="s">
         <v>142</v>
       </c>
-      <c r="AM11">
+      <c r="AN11">
         <v>5</v>
       </c>
-      <c r="AN11">
+      <c r="AO11">
         <v>200</v>
       </c>
-      <c r="AO11" s="2" t="s">
+      <c r="AP11" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="AP11">
+      <c r="AQ11">
         <v>1</v>
       </c>
-      <c r="AQ11" s="2" t="s">
+      <c r="AR11" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AR11" s="13">
+      <c r="AS11" s="13">
         <v>0.25</v>
       </c>
-      <c r="AS11" s="13">
+      <c r="AT11" s="13">
         <v>0.14499999999999999</v>
       </c>
-      <c r="AT11" s="13">
+      <c r="AU11" s="13">
         <v>0.05</v>
       </c>
-      <c r="AU11" s="19" t="b">
-        <v>0</v>
-      </c>
       <c r="AV11" s="19" t="b">
         <v>0</v>
       </c>
       <c r="AW11" s="19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AX11" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
       <c r="C12" s="27"/>
       <c r="D12" s="27"/>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>184</v>
       </c>
@@ -2397,83 +2407,83 @@
       <c r="W13">
         <v>0</v>
       </c>
-      <c r="Y13" s="27">
+      <c r="Z13" s="27">
         <v>0.03</v>
       </c>
-      <c r="Z13" s="27">
+      <c r="AA13" s="27">
         <v>0.01</v>
       </c>
-      <c r="AA13" s="27">
+      <c r="AB13" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AB13" s="27" t="s">
+      <c r="AC13" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="AC13" s="27">
+      <c r="AD13" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AD13" s="27">
-        <v>0</v>
-      </c>
-      <c r="AE13" t="s">
+      <c r="AE13" s="27">
+        <v>0</v>
+      </c>
+      <c r="AF13" t="s">
         <v>112</v>
       </c>
-      <c r="AF13" s="2" t="s">
+      <c r="AG13" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="AG13" s="2" t="s">
+      <c r="AH13" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="AH13">
+      <c r="AI13">
         <v>1</v>
       </c>
-      <c r="AI13" s="2" t="s">
+      <c r="AJ13" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="AJ13" s="18">
+      <c r="AK13" s="18">
         <v>1</v>
       </c>
-      <c r="AK13">
+      <c r="AL13">
         <v>200</v>
       </c>
-      <c r="AL13" t="s">
+      <c r="AM13" t="s">
         <v>142</v>
       </c>
-      <c r="AM13">
+      <c r="AN13">
         <v>5</v>
       </c>
-      <c r="AN13">
+      <c r="AO13">
         <v>200</v>
       </c>
-      <c r="AO13" s="2" t="s">
+      <c r="AP13" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="AP13">
+      <c r="AQ13">
         <v>1</v>
       </c>
-      <c r="AQ13" s="2" t="s">
+      <c r="AR13" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AR13" s="13">
+      <c r="AS13" s="13">
         <v>0.25</v>
       </c>
-      <c r="AS13" s="13">
+      <c r="AT13" s="13">
         <v>0.14499999999999999</v>
       </c>
-      <c r="AT13" s="13">
+      <c r="AU13" s="13">
         <v>0.05</v>
       </c>
-      <c r="AU13" s="19" t="b">
-        <v>0</v>
-      </c>
       <c r="AV13" s="19" t="b">
         <v>0</v>
       </c>
       <c r="AW13" s="19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AX13" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>185</v>
       </c>
@@ -2531,83 +2541,83 @@
       <c r="W14">
         <v>0</v>
       </c>
-      <c r="Y14" s="27">
+      <c r="Z14" s="27">
         <v>0.03</v>
       </c>
-      <c r="Z14" s="27">
+      <c r="AA14" s="27">
         <v>0.01</v>
       </c>
-      <c r="AA14" s="27">
+      <c r="AB14" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AB14" s="27" t="s">
+      <c r="AC14" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="AC14" s="27">
+      <c r="AD14" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AD14" s="27">
-        <v>0</v>
-      </c>
-      <c r="AE14" t="s">
+      <c r="AE14" s="27">
+        <v>0</v>
+      </c>
+      <c r="AF14" t="s">
         <v>112</v>
       </c>
-      <c r="AF14" s="2" t="s">
+      <c r="AG14" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="AG14" s="2" t="s">
+      <c r="AH14" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="AH14">
+      <c r="AI14">
         <v>1</v>
       </c>
-      <c r="AI14" s="2" t="s">
+      <c r="AJ14" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="AJ14" s="18">
+      <c r="AK14" s="18">
         <v>1</v>
       </c>
-      <c r="AK14">
+      <c r="AL14">
         <v>200</v>
       </c>
-      <c r="AL14" t="s">
+      <c r="AM14" t="s">
         <v>142</v>
       </c>
-      <c r="AM14">
+      <c r="AN14">
         <v>5</v>
       </c>
-      <c r="AN14">
+      <c r="AO14">
         <v>200</v>
       </c>
-      <c r="AO14" s="2" t="s">
+      <c r="AP14" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="AP14">
+      <c r="AQ14">
         <v>1</v>
       </c>
-      <c r="AQ14" s="2" t="s">
+      <c r="AR14" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AR14" s="13">
+      <c r="AS14" s="13">
         <v>0.25</v>
       </c>
-      <c r="AS14" s="13">
+      <c r="AT14" s="13">
         <v>0.14499999999999999</v>
       </c>
-      <c r="AT14" s="13">
+      <c r="AU14" s="13">
         <v>0.05</v>
       </c>
-      <c r="AU14" s="19" t="b">
-        <v>0</v>
-      </c>
       <c r="AV14" s="19" t="b">
         <v>0</v>
       </c>
       <c r="AW14" s="19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AX14" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>186</v>
       </c>
@@ -2665,86 +2675,86 @@
       <c r="W15">
         <v>0</v>
       </c>
-      <c r="Y15" s="27">
+      <c r="Z15" s="27">
         <v>0.03</v>
       </c>
-      <c r="Z15" s="27">
+      <c r="AA15" s="27">
         <v>0.01</v>
       </c>
-      <c r="AA15" s="27">
+      <c r="AB15" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AB15" s="27" t="s">
+      <c r="AC15" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="AC15" s="27">
+      <c r="AD15" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AD15" s="27">
-        <v>0</v>
-      </c>
-      <c r="AE15" t="s">
+      <c r="AE15" s="27">
+        <v>0</v>
+      </c>
+      <c r="AF15" t="s">
         <v>112</v>
       </c>
-      <c r="AF15" s="2" t="s">
+      <c r="AG15" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="AG15" s="2" t="s">
+      <c r="AH15" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="AH15">
+      <c r="AI15">
         <v>1</v>
       </c>
-      <c r="AI15" s="2" t="s">
+      <c r="AJ15" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="AJ15" s="18">
+      <c r="AK15" s="18">
         <v>1</v>
       </c>
-      <c r="AK15">
+      <c r="AL15">
         <v>200</v>
       </c>
-      <c r="AL15" t="s">
+      <c r="AM15" t="s">
         <v>142</v>
       </c>
-      <c r="AM15">
+      <c r="AN15">
         <v>5</v>
       </c>
-      <c r="AN15">
+      <c r="AO15">
         <v>200</v>
       </c>
-      <c r="AO15" s="2" t="s">
+      <c r="AP15" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="AP15">
+      <c r="AQ15">
         <v>1</v>
       </c>
-      <c r="AQ15" s="2" t="s">
+      <c r="AR15" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AR15" s="13">
+      <c r="AS15" s="13">
         <v>0.25</v>
       </c>
-      <c r="AS15" s="13">
+      <c r="AT15" s="13">
         <v>0.14499999999999999</v>
       </c>
-      <c r="AT15" s="13">
+      <c r="AU15" s="13">
         <v>0.05</v>
       </c>
-      <c r="AU15" s="19" t="b">
-        <v>0</v>
-      </c>
       <c r="AV15" s="19" t="b">
         <v>0</v>
       </c>
       <c r="AW15" s="19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AX15" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
       <c r="C16" s="11"/>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>187</v>
       </c>
@@ -2802,83 +2812,83 @@
       <c r="W17">
         <v>0</v>
       </c>
-      <c r="Y17" s="27">
+      <c r="Z17" s="27">
         <v>0.03</v>
       </c>
-      <c r="Z17" s="27">
+      <c r="AA17" s="27">
         <v>0.01</v>
       </c>
-      <c r="AA17" s="27">
+      <c r="AB17" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AB17" s="27" t="s">
+      <c r="AC17" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="AC17" s="27">
+      <c r="AD17" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AD17" s="27">
-        <v>0</v>
-      </c>
-      <c r="AE17" t="s">
+      <c r="AE17" s="27">
+        <v>0</v>
+      </c>
+      <c r="AF17" t="s">
         <v>112</v>
       </c>
-      <c r="AF17" s="2" t="s">
+      <c r="AG17" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="AG17" s="2" t="s">
+      <c r="AH17" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="AH17">
+      <c r="AI17">
         <v>1</v>
       </c>
-      <c r="AI17" s="2" t="s">
+      <c r="AJ17" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="AJ17" s="18">
+      <c r="AK17" s="18">
         <v>1</v>
       </c>
-      <c r="AK17">
+      <c r="AL17">
         <v>200</v>
       </c>
-      <c r="AL17" t="s">
+      <c r="AM17" t="s">
         <v>142</v>
       </c>
-      <c r="AM17">
+      <c r="AN17">
         <v>5</v>
       </c>
-      <c r="AN17">
+      <c r="AO17">
         <v>200</v>
       </c>
-      <c r="AO17" s="2" t="s">
+      <c r="AP17" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="AP17">
+      <c r="AQ17">
         <v>1</v>
       </c>
-      <c r="AQ17" s="2" t="s">
+      <c r="AR17" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AR17" s="13">
+      <c r="AS17" s="13">
         <v>0.25</v>
       </c>
-      <c r="AS17" s="13">
+      <c r="AT17" s="13">
         <v>0.14499999999999999</v>
       </c>
-      <c r="AT17" s="13">
+      <c r="AU17" s="13">
         <v>0.05</v>
       </c>
-      <c r="AU17" s="19" t="b">
-        <v>0</v>
-      </c>
       <c r="AV17" s="19" t="b">
         <v>0</v>
       </c>
       <c r="AW17" s="19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AX17" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>188</v>
       </c>
@@ -2936,83 +2946,83 @@
       <c r="W18">
         <v>0</v>
       </c>
-      <c r="Y18" s="27">
+      <c r="Z18" s="27">
         <v>0.03</v>
       </c>
-      <c r="Z18" s="27">
+      <c r="AA18" s="27">
         <v>0.01</v>
       </c>
-      <c r="AA18" s="27">
+      <c r="AB18" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AB18" s="27" t="s">
+      <c r="AC18" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="AC18" s="27">
+      <c r="AD18" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AD18" s="27">
-        <v>0</v>
-      </c>
-      <c r="AE18" t="s">
+      <c r="AE18" s="27">
+        <v>0</v>
+      </c>
+      <c r="AF18" t="s">
         <v>112</v>
       </c>
-      <c r="AF18" s="2" t="s">
+      <c r="AG18" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="AG18" s="2" t="s">
+      <c r="AH18" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="AH18">
+      <c r="AI18">
         <v>1</v>
       </c>
-      <c r="AI18" s="2" t="s">
+      <c r="AJ18" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="AJ18" s="18">
+      <c r="AK18" s="18">
         <v>1</v>
       </c>
-      <c r="AK18">
+      <c r="AL18">
         <v>200</v>
       </c>
-      <c r="AL18" t="s">
+      <c r="AM18" t="s">
         <v>142</v>
       </c>
-      <c r="AM18">
+      <c r="AN18">
         <v>5</v>
       </c>
-      <c r="AN18">
+      <c r="AO18">
         <v>200</v>
       </c>
-      <c r="AO18" s="2" t="s">
+      <c r="AP18" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="AP18">
+      <c r="AQ18">
         <v>1</v>
       </c>
-      <c r="AQ18" s="2" t="s">
+      <c r="AR18" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AR18" s="13">
+      <c r="AS18" s="13">
         <v>0.25</v>
       </c>
-      <c r="AS18" s="13">
+      <c r="AT18" s="13">
         <v>0.14499999999999999</v>
       </c>
-      <c r="AT18" s="13">
+      <c r="AU18" s="13">
         <v>0.05</v>
       </c>
-      <c r="AU18" s="19" t="b">
-        <v>0</v>
-      </c>
       <c r="AV18" s="19" t="b">
         <v>0</v>
       </c>
       <c r="AW18" s="19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AX18" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>189</v>
       </c>
@@ -3070,90 +3080,90 @@
       <c r="W19">
         <v>0</v>
       </c>
-      <c r="Y19" s="27">
+      <c r="Z19" s="27">
         <v>0.03</v>
       </c>
-      <c r="Z19" s="27">
+      <c r="AA19" s="27">
         <v>0.01</v>
       </c>
-      <c r="AA19" s="27">
+      <c r="AB19" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AB19" s="27" t="s">
+      <c r="AC19" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="AC19" s="27">
+      <c r="AD19" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AD19" s="27">
-        <v>0</v>
-      </c>
-      <c r="AE19" t="s">
+      <c r="AE19" s="27">
+        <v>0</v>
+      </c>
+      <c r="AF19" t="s">
         <v>112</v>
       </c>
-      <c r="AF19" s="2" t="s">
+      <c r="AG19" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="AG19" s="2" t="s">
+      <c r="AH19" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="AH19">
+      <c r="AI19">
         <v>1</v>
       </c>
-      <c r="AI19" s="2" t="s">
+      <c r="AJ19" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="AJ19" s="18">
+      <c r="AK19" s="18">
         <v>1</v>
       </c>
-      <c r="AK19">
+      <c r="AL19">
         <v>200</v>
       </c>
-      <c r="AL19" t="s">
+      <c r="AM19" t="s">
         <v>142</v>
       </c>
-      <c r="AM19">
+      <c r="AN19">
         <v>5</v>
       </c>
-      <c r="AN19">
+      <c r="AO19">
         <v>200</v>
       </c>
-      <c r="AO19" s="2" t="s">
+      <c r="AP19" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="AP19">
+      <c r="AQ19">
         <v>1</v>
       </c>
-      <c r="AQ19" s="2" t="s">
+      <c r="AR19" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AR19" s="13">
+      <c r="AS19" s="13">
         <v>0.25</v>
       </c>
-      <c r="AS19" s="13">
+      <c r="AT19" s="13">
         <v>0.14499999999999999</v>
       </c>
-      <c r="AT19" s="13">
+      <c r="AU19" s="13">
         <v>0.05</v>
       </c>
-      <c r="AU19" s="19" t="b">
-        <v>0</v>
-      </c>
       <c r="AV19" s="19" t="b">
         <v>0</v>
       </c>
       <c r="AW19" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AX19" s="19" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="AI4:AK4"/>
+    <mergeCell ref="AJ4:AL4"/>
     <mergeCell ref="P4:W4"/>
-    <mergeCell ref="Y4:AA4"/>
-    <mergeCell ref="AF4:AH4"/>
-    <mergeCell ref="AQ4:AT4"/>
-    <mergeCell ref="AB4:AD4"/>
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="AG4:AI4"/>
+    <mergeCell ref="AR4:AU4"/>
+    <mergeCell ref="AC4:AE4"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="H4:I4"/>
@@ -3161,19 +3171,19 @@
     <mergeCell ref="N4:O4"/>
   </mergeCells>
   <dataValidations count="23">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO6 AO9:AO11 AO13:AO15 AO17:AO19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP6 AP9:AP11 AP13:AP15 AP17:AP19">
       <formula1>"MA,EAA"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG6 AG9:AG11 AG13:AG15 AG17:AG19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH6 AH9:AH11 AH13:AH15 AH17:AH19">
       <formula1>"cd,cp,sl"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF6 AF9:AF11 AF13:AF15 AF17:AF19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG6 AG9:AG11 AG13:AG15 AG17:AG19">
       <formula1>"open,closed"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ6 AQ9:AQ11 AQ13:AQ15 AQ17:AQ19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR6 AR9:AR11 AR13:AR15 AR17:AR19">
       <formula1>ConPolicy</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3185,54 +3195,54 @@
       <formula1>55</formula1>
       <formula2>65</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="U6 Z6 U9:U11 Z9:Z11 U13:U15 Z13:Z15 U17:U19 Z17:Z19">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="U6 AA6 U9:U11 AA9:AA11 U13:U15 AA13:AA15 U17:U19 AA17:AA19">
       <formula1>0</formula1>
       <formula2>0.1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="W9:X19 V13:V15 V17:V19 V9:V11 V6:W6">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="W9:Y19 V13:V15 V17:V19 V9:V11 V6:W6">
       <formula1>0</formula1>
       <formula2>15</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="X6:Y6 AC6 AA6 Y9:Y11 AC9:AC11 AA9:AA11 Y13:Y15 AC13:AC15 AA13:AA15 Y17:Y19 AC17:AC19 AA17:AA19">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="X6:Z6 AD6 AB6 Z9:Z11 AD9:AD11 AB9:AB11 Z13:Z15 AD13:AD15 AB13:AB15 Z17:Z19 AD17:AD19 AB17:AB19">
       <formula1>0</formula1>
       <formula2>0.2</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AH6 AH9:AH11 AH13:AH15 AH17:AH19">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AI6 AI9:AI11 AI13:AI15 AI17:AI19">
       <formula1>0</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AR6:AS6 AR9:AS11 AR13:AS15 AR17:AS19">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AS6:AT6 AS9:AT11 AS13:AT15 AS17:AT19">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AT6 AT9:AT11 AT13:AT15 AT17:AT19">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AU6 AU9:AU11 AU13:AU15 AU17:AU19">
       <formula1>0</formula1>
       <formula2>0.3</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="AD6 AD9:AD11 AD13:AD15 AD17:AD19">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="AE6 AE9:AE11 AE13:AE15 AE17:AE19">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AM6 AM9:AM11 AM13:AM15 AM17:AM19">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AN6 AN9:AN11 AN13:AN15 AN17:AN19">
       <formula1>1</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN6 AN9:AN11 AN13:AN15 AN17:AN19">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO6 AO9:AO11 AO13:AO15 AO17:AO19">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP6 AP9:AP11 AP13:AP15 AP17:AP19">
+    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ6 AQ9:AQ11 AQ13:AQ15 AQ17:AQ19">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="AB6 AB9:AB11 AB13:AB15 AB17:AB19"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AU6:AW6 AU9:AW11 AU13:AW15 AU17:AW19">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="AC6 AC9:AC11 AC13:AC15 AC17:AC19"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AV6:AX6 AV9:AX11 AV13:AX15 AV17:AX19">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI6 AI9:AI11 AI13:AI15 AI17:AI19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ6 AJ9:AJ11 AJ13:AJ15 AJ17:AJ19">
       <formula1>"MA,AL,AL_pct"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ6 AJ9:AJ11 AJ13:AJ15 AJ17:AJ19">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK6 AK9:AK11 AK13:AK15 AK17:AK19">
       <formula1>0</formula1>
       <formula2>1.5</formula2>
     </dataValidation>
@@ -3454,8 +3464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3493,7 +3503,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <v>10</v>

</xml_diff>

<commit_message>
fixed internal consistency issue
First consistent version of MRA
</commit_message>
<xml_diff>
--- a/IO_Dev/RunControl_Dev.xlsx
+++ b/IO_Dev/RunControl_Dev.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="231">
   <si>
     <t>Sheet #</t>
   </si>
@@ -662,9 +662,6 @@
     <t>AZ-PERS</t>
   </si>
   <si>
-    <t>LA_CERA</t>
-  </si>
-  <si>
     <t>WA-PERS2</t>
   </si>
   <si>
@@ -711,6 +708,21 @@
   </si>
   <si>
     <t>term.average</t>
+  </si>
+  <si>
+    <t>AZ-PERS_F075</t>
+  </si>
+  <si>
+    <t>OH-PERS_F075</t>
+  </si>
+  <si>
+    <t>WA-PERS2_F075</t>
+  </si>
+  <si>
+    <t>LA-CERA</t>
+  </si>
+  <si>
+    <t>LA-CERA_F075</t>
   </si>
 </sst>
 </file>
@@ -924,7 +936,11 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -933,19 +949,15 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1447,18 +1459,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AX29"/>
+  <dimension ref="A1:AX31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="V6" sqref="V6"/>
+      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="2" width="67.140625" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
@@ -1536,7 +1548,7 @@
         <v>31</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="U2" s="4" t="s">
         <v>32</v>
@@ -1548,10 +1560,10 @@
         <v>34</v>
       </c>
       <c r="X2" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="Y2" s="4" t="s">
         <v>216</v>
-      </c>
-      <c r="Y2" s="4" t="s">
-        <v>217</v>
       </c>
       <c r="Z2" s="4" t="s">
         <v>35</v>
@@ -1644,66 +1656,66 @@
       </c>
     </row>
     <row r="4" spans="1:50" s="8" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="36" t="s">
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="36"/>
+      <c r="E4" s="33"/>
       <c r="F4" s="28"/>
       <c r="G4" s="28"/>
-      <c r="H4" s="37" t="s">
+      <c r="H4" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="32" t="s">
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="L4" s="32"/>
+      <c r="L4" s="34"/>
       <c r="M4" s="29"/>
-      <c r="N4" s="33" t="s">
+      <c r="N4" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="O4" s="33"/>
-      <c r="P4" s="32" t="s">
+      <c r="O4" s="35"/>
+      <c r="P4" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="32"/>
-      <c r="S4" s="32"/>
-      <c r="T4" s="32"/>
-      <c r="U4" s="32"/>
-      <c r="V4" s="32"/>
-      <c r="W4" s="32"/>
+      <c r="Q4" s="34"/>
+      <c r="R4" s="34"/>
+      <c r="S4" s="34"/>
+      <c r="T4" s="34"/>
+      <c r="U4" s="34"/>
+      <c r="V4" s="34"/>
+      <c r="W4" s="34"/>
       <c r="X4" s="30"/>
       <c r="Y4" s="30"/>
-      <c r="Z4" s="33" t="s">
+      <c r="Z4" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="AA4" s="33"/>
-      <c r="AB4" s="33"/>
-      <c r="AC4" s="31" t="s">
+      <c r="AA4" s="35"/>
+      <c r="AB4" s="35"/>
+      <c r="AC4" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="AD4" s="31"/>
-      <c r="AE4" s="31"/>
+      <c r="AD4" s="37"/>
+      <c r="AE4" s="37"/>
       <c r="AF4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AG4" s="34" t="s">
+      <c r="AG4" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="AH4" s="34"/>
-      <c r="AI4" s="34"/>
-      <c r="AJ4" s="31" t="s">
+      <c r="AH4" s="32"/>
+      <c r="AI4" s="32"/>
+      <c r="AJ4" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="AK4" s="31"/>
-      <c r="AL4" s="31"/>
+      <c r="AK4" s="37"/>
+      <c r="AL4" s="37"/>
       <c r="AM4" s="22" t="s">
         <v>70</v>
       </c>
@@ -1711,12 +1723,12 @@
       <c r="AO4" s="22"/>
       <c r="AP4" s="22"/>
       <c r="AQ4" s="22"/>
-      <c r="AR4" s="35" t="s">
+      <c r="AR4" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="AS4" s="35"/>
-      <c r="AT4" s="35"/>
-      <c r="AU4" s="35"/>
+      <c r="AS4" s="38"/>
+      <c r="AT4" s="38"/>
+      <c r="AU4" s="38"/>
       <c r="AV4" s="16"/>
       <c r="AW4" s="23"/>
       <c r="AX4" s="21"/>
@@ -1881,10 +1893,10 @@
         <v>175</v>
       </c>
       <c r="C6" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E6" t="s">
         <v>198</v>
@@ -1902,16 +1914,16 @@
         <v>109</v>
       </c>
       <c r="J6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K6" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="L6" t="s">
-        <v>205</v>
+        <v>225</v>
       </c>
       <c r="M6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="N6" s="12">
         <v>0</v>
@@ -1938,7 +1950,7 @@
         <v>0.02</v>
       </c>
       <c r="V6">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="W6">
         <v>10</v>
@@ -2036,7 +2048,7 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E8" t="s">
         <v>198</v>
@@ -2054,16 +2066,16 @@
         <v>109</v>
       </c>
       <c r="J8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K8" t="s">
         <v>147</v>
       </c>
       <c r="L8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="N8" s="27">
         <v>0</v>
@@ -2090,7 +2102,7 @@
         <v>0.02</v>
       </c>
       <c r="V8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="W8">
         <v>10</v>
@@ -2179,16 +2191,16 @@
     </row>
     <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>210</v>
+        <v>229</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>175</v>
       </c>
       <c r="C9" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
       <c r="E9" t="s">
         <v>206</v>
@@ -2197,7 +2209,7 @@
         <v>1000</v>
       </c>
       <c r="G9">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="H9" t="s">
         <v>109</v>
@@ -2206,16 +2218,16 @@
         <v>109</v>
       </c>
       <c r="J9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="K9" t="s">
         <v>147</v>
       </c>
       <c r="L9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="N9" s="27">
         <v>0</v>
@@ -2242,7 +2254,7 @@
         <v>0.02</v>
       </c>
       <c r="V9">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="W9">
         <v>10</v>
@@ -2331,7 +2343,7 @@
     </row>
     <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B10" s="20" t="s">
         <v>175</v>
@@ -2340,7 +2352,7 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E10" t="s">
         <v>207</v>
@@ -2349,7 +2361,7 @@
         <v>1000</v>
       </c>
       <c r="G10">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="H10" t="s">
         <v>109</v>
@@ -2358,16 +2370,16 @@
         <v>109</v>
       </c>
       <c r="J10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K10" t="s">
         <v>147</v>
       </c>
       <c r="L10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="N10" s="27">
         <v>0</v>
@@ -2394,7 +2406,7 @@
         <v>0.02</v>
       </c>
       <c r="V10">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="W10">
         <v>10</v>
@@ -2483,7 +2495,7 @@
     </row>
     <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B11" s="20" t="s">
         <v>175</v>
@@ -2492,7 +2504,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E11" t="s">
         <v>208</v>
@@ -2501,7 +2513,7 @@
         <v>1000</v>
       </c>
       <c r="G11">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="H11" t="s">
         <v>109</v>
@@ -2510,16 +2522,16 @@
         <v>109</v>
       </c>
       <c r="J11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K11" t="s">
         <v>147</v>
       </c>
       <c r="L11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="N11" s="27">
         <v>0</v>
@@ -2546,7 +2558,7 @@
         <v>0.02</v>
       </c>
       <c r="V11">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="W11">
         <v>10</v>
@@ -2633,277 +2645,620 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>181</v>
-      </c>
-      <c r="B19" s="20" t="s">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="C12" s="11"/>
+    </row>
+    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>226</v>
+      </c>
+      <c r="B13" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="C19" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="C13" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>221</v>
+      </c>
+      <c r="E13" t="s">
+        <v>198</v>
+      </c>
+      <c r="F13">
+        <v>1000</v>
+      </c>
+      <c r="G13">
+        <v>500</v>
+      </c>
+      <c r="H13" t="s">
         <v>109</v>
       </c>
-      <c r="E19" t="s">
+      <c r="I13" t="s">
         <v>109</v>
       </c>
-      <c r="H19" t="s">
+      <c r="J13" t="s">
+        <v>218</v>
+      </c>
+      <c r="K13" t="s">
+        <v>147</v>
+      </c>
+      <c r="L13" t="s">
+        <v>225</v>
+      </c>
+      <c r="M13" t="s">
+        <v>212</v>
+      </c>
+      <c r="N13" s="27">
+        <v>0</v>
+      </c>
+      <c r="O13" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="P13" s="27">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="Q13">
+        <v>3</v>
+      </c>
+      <c r="R13">
+        <v>75</v>
+      </c>
+      <c r="S13">
+        <v>50</v>
+      </c>
+      <c r="T13">
+        <v>60</v>
+      </c>
+      <c r="U13" s="27">
+        <v>0.02</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>10</v>
+      </c>
+      <c r="X13" s="27">
+        <v>0.04</v>
+      </c>
+      <c r="Y13" s="27">
+        <v>0.04</v>
+      </c>
+      <c r="Z13" s="27">
+        <v>0.03</v>
+      </c>
+      <c r="AA13" s="27">
+        <v>0.01</v>
+      </c>
+      <c r="AB13" s="27">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AC13" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD13" s="27">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AE13" s="27">
+        <v>0</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG13" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH13" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="AI13">
+        <v>1</v>
+      </c>
+      <c r="AJ13" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AK13" s="18">
+        <v>0.75</v>
+      </c>
+      <c r="AL13">
+        <v>200</v>
+      </c>
+      <c r="AM13" t="s">
+        <v>142</v>
+      </c>
+      <c r="AN13">
+        <v>5</v>
+      </c>
+      <c r="AO13">
+        <v>200</v>
+      </c>
+      <c r="AP13" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ13">
+        <v>1</v>
+      </c>
+      <c r="AR13" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AS13" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="AT13" s="13">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AU13" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="AV13" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AW13" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AX13" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>230</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="C14" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>206</v>
+      </c>
+      <c r="E14" t="s">
+        <v>206</v>
+      </c>
+      <c r="F14">
+        <v>1000</v>
+      </c>
+      <c r="G14">
+        <v>600</v>
+      </c>
+      <c r="H14" t="s">
         <v>109</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I14" t="s">
         <v>109</v>
       </c>
-      <c r="K19" t="s">
+      <c r="J14" t="s">
+        <v>219</v>
+      </c>
+      <c r="K14" t="s">
         <v>147</v>
       </c>
-      <c r="L19" t="s">
-        <v>168</v>
-      </c>
-      <c r="N19" s="27">
-        <v>0</v>
-      </c>
-      <c r="O19" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="P19" s="27">
+      <c r="L14" t="s">
+        <v>225</v>
+      </c>
+      <c r="M14" t="s">
+        <v>212</v>
+      </c>
+      <c r="N14" s="27">
+        <v>0</v>
+      </c>
+      <c r="O14" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="P14" s="27">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="Q19">
+      <c r="Q14">
         <v>3</v>
       </c>
-      <c r="R19">
-        <v>65</v>
-      </c>
-      <c r="S19">
-        <v>65</v>
-      </c>
-      <c r="T19">
-        <v>65</v>
-      </c>
-      <c r="U19" s="27">
+      <c r="R14">
+        <v>75</v>
+      </c>
+      <c r="S14">
+        <v>50</v>
+      </c>
+      <c r="T14">
+        <v>60</v>
+      </c>
+      <c r="U14" s="27">
         <v>0.02</v>
       </c>
-      <c r="V19">
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
         <v>10</v>
       </c>
-      <c r="W19">
-        <v>0</v>
-      </c>
-      <c r="Z19" s="27">
+      <c r="X14" s="27">
+        <v>0.04</v>
+      </c>
+      <c r="Y14" s="27">
+        <v>0.04</v>
+      </c>
+      <c r="Z14" s="27">
         <v>0.03</v>
       </c>
-      <c r="AA19" s="27">
+      <c r="AA14" s="27">
         <v>0.01</v>
       </c>
-      <c r="AB19" s="27">
+      <c r="AB14" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AC19" s="27" t="s">
+      <c r="AC14" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="AD19" s="27">
+      <c r="AD14" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AE19" s="27">
-        <v>0</v>
-      </c>
-      <c r="AF19" t="s">
+      <c r="AE14" s="27">
+        <v>0</v>
+      </c>
+      <c r="AF14" t="s">
         <v>112</v>
       </c>
-      <c r="AG19" s="2" t="s">
+      <c r="AG14" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="AH19" s="2" t="s">
+      <c r="AH14" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="AI19">
+      <c r="AI14">
         <v>1</v>
       </c>
-      <c r="AJ19" s="2" t="s">
+      <c r="AJ14" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="AK19" s="18">
+      <c r="AK14" s="18">
+        <v>0.75</v>
+      </c>
+      <c r="AL14">
+        <v>200</v>
+      </c>
+      <c r="AM14" t="s">
+        <v>142</v>
+      </c>
+      <c r="AN14">
+        <v>5</v>
+      </c>
+      <c r="AO14">
+        <v>200</v>
+      </c>
+      <c r="AP14" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ14">
         <v>1</v>
       </c>
-      <c r="AL19">
+      <c r="AR14" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AS14" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="AT14" s="13">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AU14" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="AV14" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AW14" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AX14" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>227</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="C15" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>223</v>
+      </c>
+      <c r="E15" t="s">
+        <v>207</v>
+      </c>
+      <c r="F15">
+        <v>1000</v>
+      </c>
+      <c r="G15">
+        <v>600</v>
+      </c>
+      <c r="H15" t="s">
+        <v>109</v>
+      </c>
+      <c r="I15" t="s">
+        <v>109</v>
+      </c>
+      <c r="J15" t="s">
+        <v>220</v>
+      </c>
+      <c r="K15" t="s">
+        <v>147</v>
+      </c>
+      <c r="L15" t="s">
+        <v>225</v>
+      </c>
+      <c r="M15" t="s">
+        <v>212</v>
+      </c>
+      <c r="N15" s="27">
+        <v>0</v>
+      </c>
+      <c r="O15" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="P15" s="27">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="Q15">
+        <v>3</v>
+      </c>
+      <c r="R15">
+        <v>75</v>
+      </c>
+      <c r="S15">
+        <v>50</v>
+      </c>
+      <c r="T15">
+        <v>60</v>
+      </c>
+      <c r="U15" s="27">
+        <v>0.02</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>10</v>
+      </c>
+      <c r="X15" s="27">
+        <v>0.04</v>
+      </c>
+      <c r="Y15" s="27">
+        <v>0.04</v>
+      </c>
+      <c r="Z15" s="27">
+        <v>0.03</v>
+      </c>
+      <c r="AA15" s="27">
+        <v>0.01</v>
+      </c>
+      <c r="AB15" s="27">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AC15" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD15" s="27">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AE15" s="27">
+        <v>0</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG15" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH15" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="AI15">
+        <v>1</v>
+      </c>
+      <c r="AJ15" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AK15" s="18">
+        <v>0.75</v>
+      </c>
+      <c r="AL15">
         <v>200</v>
       </c>
-      <c r="AM19" t="s">
+      <c r="AM15" t="s">
         <v>142</v>
       </c>
-      <c r="AN19">
+      <c r="AN15">
         <v>5</v>
       </c>
-      <c r="AO19">
+      <c r="AO15">
         <v>200</v>
       </c>
-      <c r="AP19" s="2" t="s">
+      <c r="AP15" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="AQ19">
+      <c r="AQ15">
         <v>1</v>
       </c>
-      <c r="AR19" s="2" t="s">
+      <c r="AR15" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AS19" s="13">
+      <c r="AS15" s="13">
         <v>0.25</v>
       </c>
-      <c r="AT19" s="13">
+      <c r="AT15" s="13">
         <v>0.14499999999999999</v>
       </c>
-      <c r="AU19" s="13">
+      <c r="AU15" s="13">
         <v>0.05</v>
       </c>
-      <c r="AV19" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="AW19" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="AX19" s="19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>182</v>
-      </c>
-      <c r="B20" s="20" t="s">
+      <c r="AV15" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AW15" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AX15" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>228</v>
+      </c>
+      <c r="B16" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="C20" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="D20" t="s">
-        <v>171</v>
-      </c>
-      <c r="E20" t="s">
-        <v>171</v>
-      </c>
-      <c r="H20" t="s">
+      <c r="C16" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>224</v>
+      </c>
+      <c r="E16" t="s">
+        <v>208</v>
+      </c>
+      <c r="F16">
+        <v>1000</v>
+      </c>
+      <c r="G16">
+        <v>300</v>
+      </c>
+      <c r="H16" t="s">
         <v>109</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I16" t="s">
         <v>109</v>
       </c>
-      <c r="K20" t="s">
+      <c r="J16" t="s">
+        <v>217</v>
+      </c>
+      <c r="K16" t="s">
         <v>147</v>
       </c>
-      <c r="L20" t="s">
-        <v>168</v>
-      </c>
-      <c r="N20" s="27">
-        <v>0</v>
-      </c>
-      <c r="O20" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="P20" s="27">
+      <c r="L16" t="s">
+        <v>225</v>
+      </c>
+      <c r="M16" t="s">
+        <v>212</v>
+      </c>
+      <c r="N16" s="27">
+        <v>0</v>
+      </c>
+      <c r="O16" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="P16" s="27">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="Q20">
+      <c r="Q16">
         <v>3</v>
       </c>
-      <c r="R20">
-        <v>65</v>
-      </c>
-      <c r="S20">
-        <v>65</v>
-      </c>
-      <c r="T20">
-        <v>65</v>
-      </c>
-      <c r="U20" s="27">
+      <c r="R16">
+        <v>75</v>
+      </c>
+      <c r="S16">
+        <v>50</v>
+      </c>
+      <c r="T16">
+        <v>60</v>
+      </c>
+      <c r="U16" s="27">
         <v>0.02</v>
       </c>
-      <c r="V20">
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
         <v>10</v>
       </c>
-      <c r="W20">
-        <v>0</v>
-      </c>
-      <c r="Z20" s="27">
+      <c r="X16" s="27">
+        <v>0.04</v>
+      </c>
+      <c r="Y16" s="27">
+        <v>0.04</v>
+      </c>
+      <c r="Z16" s="27">
         <v>0.03</v>
       </c>
-      <c r="AA20" s="27">
+      <c r="AA16" s="27">
         <v>0.01</v>
       </c>
-      <c r="AB20" s="27">
+      <c r="AB16" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AC20" s="27" t="s">
+      <c r="AC16" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="AD20" s="27">
+      <c r="AD16" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AE20" s="27">
-        <v>0</v>
-      </c>
-      <c r="AF20" t="s">
+      <c r="AE16" s="27">
+        <v>0</v>
+      </c>
+      <c r="AF16" t="s">
         <v>112</v>
       </c>
-      <c r="AG20" s="2" t="s">
+      <c r="AG16" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="AH20" s="2" t="s">
+      <c r="AH16" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="AI20">
+      <c r="AI16">
         <v>1</v>
       </c>
-      <c r="AJ20" s="2" t="s">
+      <c r="AJ16" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="AK20" s="18">
+      <c r="AK16" s="18">
+        <v>0.75</v>
+      </c>
+      <c r="AL16">
+        <v>200</v>
+      </c>
+      <c r="AM16" t="s">
+        <v>142</v>
+      </c>
+      <c r="AN16">
+        <v>5</v>
+      </c>
+      <c r="AO16">
+        <v>200</v>
+      </c>
+      <c r="AP16" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ16">
         <v>1</v>
       </c>
-      <c r="AL20">
-        <v>200</v>
-      </c>
-      <c r="AM20" t="s">
-        <v>142</v>
-      </c>
-      <c r="AN20">
-        <v>5</v>
-      </c>
-      <c r="AO20">
-        <v>200</v>
-      </c>
-      <c r="AP20" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AQ20">
-        <v>1</v>
-      </c>
-      <c r="AR20" s="2" t="s">
+      <c r="AR16" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AS20" s="13">
+      <c r="AS16" s="13">
         <v>0.25</v>
       </c>
-      <c r="AT20" s="13">
+      <c r="AT16" s="13">
         <v>0.14499999999999999</v>
       </c>
-      <c r="AU20" s="13">
+      <c r="AU16" s="13">
         <v>0.05</v>
       </c>
-      <c r="AV20" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="AW20" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="AX20" s="19" t="b">
+      <c r="AV16" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AW16" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AX16" s="19" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B21" s="20" t="s">
         <v>175</v>
@@ -2912,10 +3267,10 @@
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>172</v>
+        <v>109</v>
       </c>
       <c r="E21" t="s">
-        <v>172</v>
+        <v>109</v>
       </c>
       <c r="H21" t="s">
         <v>109</v>
@@ -3036,12 +3391,142 @@
       </c>
     </row>
     <row r="22" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
+      <c r="A22" t="s">
+        <v>182</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="C22" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>171</v>
+      </c>
+      <c r="E22" t="s">
+        <v>171</v>
+      </c>
+      <c r="H22" t="s">
+        <v>109</v>
+      </c>
+      <c r="I22" t="s">
+        <v>109</v>
+      </c>
+      <c r="K22" t="s">
+        <v>147</v>
+      </c>
+      <c r="L22" t="s">
+        <v>168</v>
+      </c>
+      <c r="N22" s="27">
+        <v>0</v>
+      </c>
+      <c r="O22" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="P22" s="27">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="Q22">
+        <v>3</v>
+      </c>
+      <c r="R22">
+        <v>65</v>
+      </c>
+      <c r="S22">
+        <v>65</v>
+      </c>
+      <c r="T22">
+        <v>65</v>
+      </c>
+      <c r="U22" s="27">
+        <v>0.02</v>
+      </c>
+      <c r="V22">
+        <v>10</v>
+      </c>
+      <c r="W22">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="27">
+        <v>0.03</v>
+      </c>
+      <c r="AA22" s="27">
+        <v>0.01</v>
+      </c>
+      <c r="AB22" s="27">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AC22" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD22" s="27">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AE22" s="27">
+        <v>0</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG22" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH22" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="AI22">
+        <v>1</v>
+      </c>
+      <c r="AJ22" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AK22" s="18">
+        <v>1</v>
+      </c>
+      <c r="AL22">
+        <v>200</v>
+      </c>
+      <c r="AM22" t="s">
+        <v>142</v>
+      </c>
+      <c r="AN22">
+        <v>5</v>
+      </c>
+      <c r="AO22">
+        <v>200</v>
+      </c>
+      <c r="AP22" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ22">
+        <v>1</v>
+      </c>
+      <c r="AR22" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AS22" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="AT22" s="13">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AU22" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="AV22" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AW22" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AX22" s="19" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B23" s="20" t="s">
         <v>175</v>
@@ -3050,10 +3535,10 @@
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>109</v>
+        <v>172</v>
       </c>
       <c r="E23" t="s">
-        <v>109</v>
+        <v>172</v>
       </c>
       <c r="H23" t="s">
         <v>109</v>
@@ -3083,7 +3568,7 @@
         <v>65</v>
       </c>
       <c r="S23">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="T23">
         <v>65</v>
@@ -3174,142 +3659,12 @@
       </c>
     </row>
     <row r="24" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>185</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>175</v>
-      </c>
-      <c r="C24" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="D24" t="s">
-        <v>171</v>
-      </c>
-      <c r="E24" t="s">
-        <v>171</v>
-      </c>
-      <c r="H24" t="s">
-        <v>109</v>
-      </c>
-      <c r="I24" t="s">
-        <v>109</v>
-      </c>
-      <c r="K24" t="s">
-        <v>147</v>
-      </c>
-      <c r="L24" t="s">
-        <v>168</v>
-      </c>
-      <c r="N24" s="27">
-        <v>0</v>
-      </c>
-      <c r="O24" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="P24" s="27">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="Q24">
-        <v>3</v>
-      </c>
-      <c r="R24">
-        <v>65</v>
-      </c>
-      <c r="S24">
-        <v>55</v>
-      </c>
-      <c r="T24">
-        <v>65</v>
-      </c>
-      <c r="U24" s="27">
-        <v>0.02</v>
-      </c>
-      <c r="V24">
-        <v>10</v>
-      </c>
-      <c r="W24">
-        <v>0</v>
-      </c>
-      <c r="Z24" s="27">
-        <v>0.03</v>
-      </c>
-      <c r="AA24" s="27">
-        <v>0.01</v>
-      </c>
-      <c r="AB24" s="27">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="AC24" s="27" t="s">
-        <v>156</v>
-      </c>
-      <c r="AD24" s="27">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="AE24" s="27">
-        <v>0</v>
-      </c>
-      <c r="AF24" t="s">
-        <v>112</v>
-      </c>
-      <c r="AG24" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="AH24" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="AI24">
-        <v>1</v>
-      </c>
-      <c r="AJ24" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="AK24" s="18">
-        <v>1</v>
-      </c>
-      <c r="AL24">
-        <v>200</v>
-      </c>
-      <c r="AM24" t="s">
-        <v>142</v>
-      </c>
-      <c r="AN24">
-        <v>5</v>
-      </c>
-      <c r="AO24">
-        <v>200</v>
-      </c>
-      <c r="AP24" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AQ24">
-        <v>1</v>
-      </c>
-      <c r="AR24" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="AS24" s="13">
-        <v>0.25</v>
-      </c>
-      <c r="AT24" s="13">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="AU24" s="13">
-        <v>0.05</v>
-      </c>
-      <c r="AV24" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="AW24" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="AX24" s="19" t="b">
-        <v>0</v>
-      </c>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
     </row>
     <row r="25" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B25" s="20" t="s">
         <v>175</v>
@@ -3318,10 +3673,10 @@
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>172</v>
+        <v>109</v>
       </c>
       <c r="E25" t="s">
-        <v>172</v>
+        <v>109</v>
       </c>
       <c r="H25" t="s">
         <v>109</v>
@@ -3442,11 +3797,142 @@
       </c>
     </row>
     <row r="26" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="C26" s="11"/>
+      <c r="A26" t="s">
+        <v>185</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="C26" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" t="s">
+        <v>171</v>
+      </c>
+      <c r="E26" t="s">
+        <v>171</v>
+      </c>
+      <c r="H26" t="s">
+        <v>109</v>
+      </c>
+      <c r="I26" t="s">
+        <v>109</v>
+      </c>
+      <c r="K26" t="s">
+        <v>147</v>
+      </c>
+      <c r="L26" t="s">
+        <v>168</v>
+      </c>
+      <c r="N26" s="27">
+        <v>0</v>
+      </c>
+      <c r="O26" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="P26" s="27">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="Q26">
+        <v>3</v>
+      </c>
+      <c r="R26">
+        <v>65</v>
+      </c>
+      <c r="S26">
+        <v>55</v>
+      </c>
+      <c r="T26">
+        <v>65</v>
+      </c>
+      <c r="U26" s="27">
+        <v>0.02</v>
+      </c>
+      <c r="V26">
+        <v>10</v>
+      </c>
+      <c r="W26">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="27">
+        <v>0.03</v>
+      </c>
+      <c r="AA26" s="27">
+        <v>0.01</v>
+      </c>
+      <c r="AB26" s="27">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AC26" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD26" s="27">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AE26" s="27">
+        <v>0</v>
+      </c>
+      <c r="AF26" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG26" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH26" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="AI26">
+        <v>1</v>
+      </c>
+      <c r="AJ26" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AK26" s="18">
+        <v>1</v>
+      </c>
+      <c r="AL26">
+        <v>200</v>
+      </c>
+      <c r="AM26" t="s">
+        <v>142</v>
+      </c>
+      <c r="AN26">
+        <v>5</v>
+      </c>
+      <c r="AO26">
+        <v>200</v>
+      </c>
+      <c r="AP26" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ26">
+        <v>1</v>
+      </c>
+      <c r="AR26" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AS26" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="AT26" s="13">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AU26" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="AV26" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AW26" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AX26" s="19" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B27" s="20" t="s">
         <v>175</v>
@@ -3455,10 +3941,10 @@
         <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>109</v>
+        <v>172</v>
       </c>
       <c r="E27" t="s">
-        <v>109</v>
+        <v>172</v>
       </c>
       <c r="H27" t="s">
         <v>109</v>
@@ -3579,142 +4065,11 @@
       </c>
     </row>
     <row r="28" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>188</v>
-      </c>
-      <c r="B28" s="20" t="s">
-        <v>175</v>
-      </c>
-      <c r="C28" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="D28" t="s">
-        <v>171</v>
-      </c>
-      <c r="E28" t="s">
-        <v>171</v>
-      </c>
-      <c r="H28" t="s">
-        <v>109</v>
-      </c>
-      <c r="I28" t="s">
-        <v>109</v>
-      </c>
-      <c r="K28" t="s">
-        <v>147</v>
-      </c>
-      <c r="L28" t="s">
-        <v>168</v>
-      </c>
-      <c r="N28" s="27">
-        <v>0</v>
-      </c>
-      <c r="O28" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="P28" s="27">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="Q28">
-        <v>3</v>
-      </c>
-      <c r="R28">
-        <v>65</v>
-      </c>
-      <c r="S28">
-        <v>55</v>
-      </c>
-      <c r="T28">
-        <v>65</v>
-      </c>
-      <c r="U28" s="27">
-        <v>0.02</v>
-      </c>
-      <c r="V28">
-        <v>10</v>
-      </c>
-      <c r="W28">
-        <v>0</v>
-      </c>
-      <c r="Z28" s="27">
-        <v>0.03</v>
-      </c>
-      <c r="AA28" s="27">
-        <v>0.01</v>
-      </c>
-      <c r="AB28" s="27">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="AC28" s="27" t="s">
-        <v>156</v>
-      </c>
-      <c r="AD28" s="27">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="AE28" s="27">
-        <v>0</v>
-      </c>
-      <c r="AF28" t="s">
-        <v>112</v>
-      </c>
-      <c r="AG28" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="AH28" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="AI28">
-        <v>1</v>
-      </c>
-      <c r="AJ28" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="AK28" s="18">
-        <v>1</v>
-      </c>
-      <c r="AL28">
-        <v>200</v>
-      </c>
-      <c r="AM28" t="s">
-        <v>142</v>
-      </c>
-      <c r="AN28">
-        <v>5</v>
-      </c>
-      <c r="AO28">
-        <v>200</v>
-      </c>
-      <c r="AP28" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AQ28">
-        <v>1</v>
-      </c>
-      <c r="AR28" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="AS28" s="13">
-        <v>0.25</v>
-      </c>
-      <c r="AT28" s="13">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="AU28" s="13">
-        <v>0.05</v>
-      </c>
-      <c r="AV28" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="AW28" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="AX28" s="19" t="b">
-        <v>0</v>
-      </c>
+      <c r="C28" s="11"/>
     </row>
     <row r="29" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B29" s="20" t="s">
         <v>175</v>
@@ -3723,10 +4078,10 @@
         <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>172</v>
+        <v>109</v>
       </c>
       <c r="E29" t="s">
-        <v>172</v>
+        <v>109</v>
       </c>
       <c r="H29" t="s">
         <v>109</v>
@@ -3846,114 +4201,376 @@
         <v>0</v>
       </c>
     </row>
+    <row r="30" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>188</v>
+      </c>
+      <c r="B30" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="C30" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D30" t="s">
+        <v>171</v>
+      </c>
+      <c r="E30" t="s">
+        <v>171</v>
+      </c>
+      <c r="H30" t="s">
+        <v>109</v>
+      </c>
+      <c r="I30" t="s">
+        <v>109</v>
+      </c>
+      <c r="K30" t="s">
+        <v>147</v>
+      </c>
+      <c r="L30" t="s">
+        <v>168</v>
+      </c>
+      <c r="N30" s="27">
+        <v>0</v>
+      </c>
+      <c r="O30" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="P30" s="27">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="Q30">
+        <v>3</v>
+      </c>
+      <c r="R30">
+        <v>65</v>
+      </c>
+      <c r="S30">
+        <v>55</v>
+      </c>
+      <c r="T30">
+        <v>65</v>
+      </c>
+      <c r="U30" s="27">
+        <v>0.02</v>
+      </c>
+      <c r="V30">
+        <v>10</v>
+      </c>
+      <c r="W30">
+        <v>0</v>
+      </c>
+      <c r="Z30" s="27">
+        <v>0.03</v>
+      </c>
+      <c r="AA30" s="27">
+        <v>0.01</v>
+      </c>
+      <c r="AB30" s="27">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AC30" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD30" s="27">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AE30" s="27">
+        <v>0</v>
+      </c>
+      <c r="AF30" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG30" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH30" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="AI30">
+        <v>1</v>
+      </c>
+      <c r="AJ30" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AK30" s="18">
+        <v>1</v>
+      </c>
+      <c r="AL30">
+        <v>200</v>
+      </c>
+      <c r="AM30" t="s">
+        <v>142</v>
+      </c>
+      <c r="AN30">
+        <v>5</v>
+      </c>
+      <c r="AO30">
+        <v>200</v>
+      </c>
+      <c r="AP30" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ30">
+        <v>1</v>
+      </c>
+      <c r="AR30" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AS30" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="AT30" s="13">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AU30" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="AV30" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AW30" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AX30" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>189</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="C31" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D31" t="s">
+        <v>172</v>
+      </c>
+      <c r="E31" t="s">
+        <v>172</v>
+      </c>
+      <c r="H31" t="s">
+        <v>109</v>
+      </c>
+      <c r="I31" t="s">
+        <v>109</v>
+      </c>
+      <c r="K31" t="s">
+        <v>147</v>
+      </c>
+      <c r="L31" t="s">
+        <v>168</v>
+      </c>
+      <c r="N31" s="27">
+        <v>0</v>
+      </c>
+      <c r="O31" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="P31" s="27">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="Q31">
+        <v>3</v>
+      </c>
+      <c r="R31">
+        <v>65</v>
+      </c>
+      <c r="S31">
+        <v>55</v>
+      </c>
+      <c r="T31">
+        <v>65</v>
+      </c>
+      <c r="U31" s="27">
+        <v>0.02</v>
+      </c>
+      <c r="V31">
+        <v>10</v>
+      </c>
+      <c r="W31">
+        <v>0</v>
+      </c>
+      <c r="Z31" s="27">
+        <v>0.03</v>
+      </c>
+      <c r="AA31" s="27">
+        <v>0.01</v>
+      </c>
+      <c r="AB31" s="27">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AC31" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD31" s="27">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AE31" s="27">
+        <v>0</v>
+      </c>
+      <c r="AF31" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG31" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH31" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="AI31">
+        <v>1</v>
+      </c>
+      <c r="AJ31" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AK31" s="18">
+        <v>1</v>
+      </c>
+      <c r="AL31">
+        <v>200</v>
+      </c>
+      <c r="AM31" t="s">
+        <v>142</v>
+      </c>
+      <c r="AN31">
+        <v>5</v>
+      </c>
+      <c r="AO31">
+        <v>200</v>
+      </c>
+      <c r="AP31" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ31">
+        <v>1</v>
+      </c>
+      <c r="AR31" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AS31" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="AT31" s="13">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AU31" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="AV31" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AW31" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AX31" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="H4:J4"/>
     <mergeCell ref="AJ4:AL4"/>
     <mergeCell ref="P4:W4"/>
     <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="AG4:AI4"/>
     <mergeCell ref="AR4:AU4"/>
     <mergeCell ref="AC4:AE4"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="H4:J4"/>
   </mergeCells>
-  <dataValidations count="26">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP6 AP19:AP21 AP23:AP25 AP27:AP29 AP8:AP11">
+  <dataValidations count="24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP6 AP21:AP23 AP25:AP27 AP29:AP31 AP8:AP11 AP13:AP16">
       <formula1>"MA,EAA"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH6 AH19:AH21 AH23:AH25 AH27:AH29 AH8:AH11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH6 AH21:AH23 AH25:AH27 AH29:AH31 AH8:AH11 AH13:AH16">
       <formula1>"cd,cp,sl"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG6 AG19:AG21 AG23:AG25 AG27:AG29 AG8:AG11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG6 AG21:AG23 AG25:AG27 AG29:AG31 AG8:AG11 AG13:AG16">
       <formula1>"open,closed"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR6 AR19:AR21 AR23:AR25 AR27:AR29 AR8:AR11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR6 AR21:AR23 AR25:AR27 AR29:AR31 AR8:AR11 AR13:AR16">
       <formula1>ConPolicy</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O6 C6 O19:O21 C19:C21 O23:O25 O27:O29 C23:C29 O8:O11 C8:C11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O6 C6 O21:O23 C21:C23 O25:O27 O29:O31 C25:C31 O8:O11 O13:O16 C8:C16">
       <formula1>"TRUE,FALSE"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer 55 to 65, please" sqref="R19:S21 R27:R29 R23:R25">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer 55 to 65, please" sqref="R21:S23 R29:R31 R25:R27">
       <formula1>55</formula1>
       <formula2>65</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="U6 AA6 U19:U21 AA19:AA21 U23:U25 AA23:AA25 U27:U29 AA27:AA29 AA8:AA11 U8:U11">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="U6 AA6 U21:U23 AA21:AA23 U25:U27 AA25:AA27 U29:U31 AA29:AA31 AA8:AA11 U8:U11 AA13:AA16 U13:U16">
       <formula1>0</formula1>
       <formula2>0.1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="W19:Y29 V23:V25 V27:V29 V19:V21 V6:W6 V8:W11">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="W21:Y31 V25:V27 V29:V31 V21:V23 V6:W6 V8:W11 V13:W16">
       <formula1>0</formula1>
       <formula2>15</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="X6:Z6 AD6 AB6 Z19:Z21 AD19:AD21 AB19:AB21 Z23:Z25 AD23:AD25 AB23:AB25 Z27:Z29 AD27:AD29 AB27:AB29 X8:Z11 AB8:AB11 AD8:AD11">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="X6:Z6 AD6 AB6 Z21:Z23 AD21:AD23 AB21:AB23 Z25:Z27 AD25:AD27 AB25:AB27 Z29:Z31 AD29:AD31 AB29:AB31 X8:Z11 AB8:AB11 AD8:AD11 X13:Z16 AB13:AB16 AD13:AD16">
       <formula1>0</formula1>
       <formula2>0.2</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AI6 AI19:AI21 AI23:AI25 AI27:AI29 AI8:AI11">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AI6 AI21:AI23 AI25:AI27 AI29:AI31 AI8:AI11 AI13:AI16">
       <formula1>0</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AS6:AT6 AS19:AT21 AS23:AT25 AS27:AT29 AS8:AT11">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AS6:AT6 AS21:AT23 AS25:AT27 AS29:AT31 AS8:AT11 AS13:AT16">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AU6 AU19:AU21 AU23:AU25 AU27:AU29 AU8:AU11">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AU6 AU21:AU23 AU25:AU27 AU29:AU31 AU8:AU11 AU13:AU16">
       <formula1>0</formula1>
       <formula2>0.3</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="AE6 AE19:AE21 AE23:AE25 AE27:AE29 AE8:AE11">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="AE6 AE21:AE23 AE25:AE27 AE29:AE31 AE8:AE11 AE13:AE16">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AN6 AN19:AN21 AN23:AN25 AN27:AN29 AN8:AN11">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AN6 AN21:AN23 AN25:AN27 AN29:AN31 AN8:AN11 AN13:AN16">
       <formula1>1</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO6 AO19:AO21 AO23:AO25 AO27:AO29 AO8:AO11">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO6 AO21:AO23 AO25:AO27 AO29:AO31 AO8:AO11 AO13:AO16">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ6 AQ19:AQ21 AQ23:AQ25 AQ27:AQ29 AQ8:AQ11">
+    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ6 AQ21:AQ23 AQ25:AQ27 AQ29:AQ31 AQ8:AQ11 AQ13:AQ16">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="AC6 AC19:AC21 AC23:AC25 AC27:AC29 AC8:AC11"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AV6:AX6 AV19:AX21 AV23:AX25 AV27:AX29 AV8:AX11">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="AC6 AC21:AC23 AC25:AC27 AC29:AC31 AC8:AC11 AC13:AC16"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AV6:AX6 AV21:AX23 AV25:AX27 AV29:AX31 AV8:AX11 AV13:AX16">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ6 AJ19:AJ21 AJ23:AJ25 AJ27:AJ29 AJ8:AJ11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ6 AJ21:AJ23 AJ25:AJ27 AJ29:AJ31 AJ8:AJ11 AJ13:AJ16">
       <formula1>"MA,AL,AL_pct"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK6 AK19:AK21 AK23:AK25 AK27:AK29 AK8:AK11">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK6 AK21:AK23 AK25:AK27 AK29:AK31 AK8:AK11 AK13:AK16">
       <formula1>0</formula1>
       <formula2>1.5</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer 55 to 65, please" sqref="R6 R8:R11">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer 55 to 65, please" sqref="R6 R8:R11 R13:R16">
       <formula1>35</formula1>
       <formula2>80</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K19:K21 K23:K25 K27:K29">
-      <formula1>$A$44:$A$48</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K21:K23 K25:K27 K29:K31">
+      <formula1>$A$46:$A$50</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L19:M21 L23:M25">
-      <formula1>$A$51:$A$53</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L21:M23 L25:M27">
+      <formula1>$A$53:$A$55</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D23:J25">
-      <formula1>$A$19:$A$24</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D19:J21">
-      <formula1>$A$19:$A$24</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6:I6 H8:I11">
-      <formula1>$A$19:$A$24</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D25:J27 D21:J23 H6:I6 H8:I11 H13:I16">
+      <formula1>$A$21:$A$26</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -3965,49 +4582,49 @@
           <x14:formula1>
             <xm:f>DropDowns!$A$57:$A$61</xm:f>
           </x14:formula1>
-          <xm:sqref>K6 K8:K11</xm:sqref>
+          <xm:sqref>K6 K8:K11 K13:K16</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$69:$A$71</xm:f>
           </x14:formula1>
-          <xm:sqref>L27:M29</xm:sqref>
+          <xm:sqref>L29:M31</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$74:$A$77</xm:f>
           </x14:formula1>
-          <xm:sqref>M6:M11</xm:sqref>
+          <xm:sqref>M6:M11 M13:M16</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$64:$A$71</xm:f>
           </x14:formula1>
-          <xm:sqref>L6 L8:L11</xm:sqref>
+          <xm:sqref>L6 L8:L11 L13:L16</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$37:$A$42</xm:f>
           </x14:formula1>
-          <xm:sqref>D27:J29</xm:sqref>
+          <xm:sqref>D29:J31</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$45:$A$52</xm:f>
           </x14:formula1>
-          <xm:sqref>E6 E8:E11</xm:sqref>
+          <xm:sqref>E6 E8:E11 E13:E16</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$29:$A$42</xm:f>
           </x14:formula1>
-          <xm:sqref>D6 D8:D11</xm:sqref>
+          <xm:sqref>D6 D8:D11 D13:D16</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$21:$A$24</xm:f>
           </x14:formula1>
-          <xm:sqref>J6 J8:J11</xm:sqref>
+          <xm:sqref>J6 J8:J11 J13:J16</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4170,7 +4787,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4208,7 +4825,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="B3">
         <v>10</v>
@@ -4360,22 +4977,22 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -4415,22 +5032,22 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -4561,9 +5178,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="64" spans="1:3" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="24" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -4611,10 +5228,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>212</v>
+      </c>
+      <c r="C74" t="s">
         <v>213</v>
-      </c>
-      <c r="C74" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
bug fixes and population check
</commit_message>
<xml_diff>
--- a/IO_Dev/RunControl_Dev.xlsx
+++ b/IO_Dev/RunControl_Dev.xlsx
@@ -1465,7 +1465,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2349,7 +2349,7 @@
         <v>175</v>
       </c>
       <c r="C10" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" t="s">
         <v>223</v>
@@ -2501,7 +2501,7 @@
         <v>175</v>
       </c>
       <c r="C11" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" t="s">
         <v>224</v>
@@ -2808,7 +2808,7 @@
         <v>175</v>
       </c>
       <c r="C14" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" t="s">
         <v>206</v>

</xml_diff>

<commit_message>
fix bug in population
</commit_message>
<xml_diff>
--- a/IO_Dev/RunControl_Dev.xlsx
+++ b/IO_Dev/RunControl_Dev.xlsx
@@ -937,10 +937,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -949,13 +946,16 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1465,7 +1465,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9:C11"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1656,66 +1656,66 @@
       </c>
     </row>
     <row r="4" spans="1:50" s="8" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="33" t="s">
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="33"/>
+      <c r="E4" s="37"/>
       <c r="F4" s="28"/>
       <c r="G4" s="28"/>
-      <c r="H4" s="36" t="s">
+      <c r="H4" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="34" t="s">
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="L4" s="34"/>
+      <c r="L4" s="33"/>
       <c r="M4" s="29"/>
-      <c r="N4" s="35" t="s">
+      <c r="N4" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="O4" s="35"/>
-      <c r="P4" s="34" t="s">
+      <c r="O4" s="34"/>
+      <c r="P4" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="Q4" s="34"/>
-      <c r="R4" s="34"/>
-      <c r="S4" s="34"/>
-      <c r="T4" s="34"/>
-      <c r="U4" s="34"/>
-      <c r="V4" s="34"/>
-      <c r="W4" s="34"/>
+      <c r="Q4" s="33"/>
+      <c r="R4" s="33"/>
+      <c r="S4" s="33"/>
+      <c r="T4" s="33"/>
+      <c r="U4" s="33"/>
+      <c r="V4" s="33"/>
+      <c r="W4" s="33"/>
       <c r="X4" s="30"/>
       <c r="Y4" s="30"/>
-      <c r="Z4" s="35" t="s">
+      <c r="Z4" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="AA4" s="35"/>
-      <c r="AB4" s="35"/>
-      <c r="AC4" s="37" t="s">
+      <c r="AA4" s="34"/>
+      <c r="AB4" s="34"/>
+      <c r="AC4" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="AD4" s="37"/>
-      <c r="AE4" s="37"/>
+      <c r="AD4" s="32"/>
+      <c r="AE4" s="32"/>
       <c r="AF4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AG4" s="32" t="s">
+      <c r="AG4" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="AH4" s="32"/>
-      <c r="AI4" s="32"/>
-      <c r="AJ4" s="37" t="s">
+      <c r="AH4" s="35"/>
+      <c r="AI4" s="35"/>
+      <c r="AJ4" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="AK4" s="37"/>
-      <c r="AL4" s="37"/>
+      <c r="AK4" s="32"/>
+      <c r="AL4" s="32"/>
       <c r="AM4" s="22" t="s">
         <v>70</v>
       </c>
@@ -1723,12 +1723,12 @@
       <c r="AO4" s="22"/>
       <c r="AP4" s="22"/>
       <c r="AQ4" s="22"/>
-      <c r="AR4" s="38" t="s">
+      <c r="AR4" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="AS4" s="38"/>
-      <c r="AT4" s="38"/>
-      <c r="AU4" s="38"/>
+      <c r="AS4" s="36"/>
+      <c r="AT4" s="36"/>
+      <c r="AU4" s="36"/>
       <c r="AV4" s="16"/>
       <c r="AW4" s="23"/>
       <c r="AX4" s="21"/>
@@ -2045,7 +2045,7 @@
         <v>175</v>
       </c>
       <c r="C8" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
         <v>221</v>
@@ -2197,7 +2197,7 @@
         <v>175</v>
       </c>
       <c r="C9" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" t="s">
         <v>206</v>
@@ -2349,7 +2349,7 @@
         <v>175</v>
       </c>
       <c r="C10" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" t="s">
         <v>223</v>
@@ -2501,7 +2501,7 @@
         <v>175</v>
       </c>
       <c r="C11" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
         <v>224</v>
@@ -4471,17 +4471,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="H4:J4"/>
     <mergeCell ref="AJ4:AL4"/>
     <mergeCell ref="P4:W4"/>
     <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="AG4:AI4"/>
     <mergeCell ref="AR4:AU4"/>
     <mergeCell ref="AC4:AE4"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="H4:J4"/>
   </mergeCells>
   <dataValidations count="24">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP6 AP21:AP23 AP25:AP27 AP29:AP31 AP8:AP11 AP13:AP16">
@@ -4787,7 +4787,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add tailoring function to import_plan module
</commit_message>
<xml_diff>
--- a/IO_Dev/RunControl_Dev.xlsx
+++ b/IO_Dev/RunControl_Dev.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="7230" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="7230" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -1461,7 +1461,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AX31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
@@ -4786,7 +4786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
track new entrants as % of workforce
</commit_message>
<xml_diff>
--- a/IO_Dev/RunControl_Dev.xlsx
+++ b/IO_Dev/RunControl_Dev.xlsx
@@ -1462,10 +1462,10 @@
   <dimension ref="A1:AX31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomRight" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2045,7 +2045,7 @@
         <v>175</v>
       </c>
       <c r="C8" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
         <v>221</v>
@@ -2197,7 +2197,7 @@
         <v>175</v>
       </c>
       <c r="C9" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
         <v>222</v>
@@ -2501,7 +2501,7 @@
         <v>175</v>
       </c>
       <c r="C11" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" t="s">
         <v>224</v>
@@ -4582,7 +4582,7 @@
           <x14:formula1>
             <xm:f>DropDowns!$A$57:$A$61</xm:f>
           </x14:formula1>
-          <xm:sqref>K6 K8:K11 K13:K16</xm:sqref>
+          <xm:sqref>K6 K13:K16 K8:K11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>

<commit_message>
track inactive terms and terms in benefit status
</commit_message>
<xml_diff>
--- a/IO_Dev/RunControl_Dev.xlsx
+++ b/IO_Dev/RunControl_Dev.xlsx
@@ -1465,7 +1465,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="N9" sqref="N9"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2045,7 +2045,7 @@
         <v>175</v>
       </c>
       <c r="C8" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" t="s">
         <v>221</v>
@@ -2078,7 +2078,7 @@
         <v>212</v>
       </c>
       <c r="N8" s="27">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="O8" s="19" t="b">
         <v>0</v>
@@ -2349,7 +2349,7 @@
         <v>175</v>
       </c>
       <c r="C10" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" t="s">
         <v>223</v>
@@ -2501,7 +2501,7 @@
         <v>175</v>
       </c>
       <c r="C11" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" t="s">
         <v>224</v>
@@ -4787,7 +4787,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4825,7 +4825,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B3">
         <v>10</v>

</xml_diff>

<commit_message>
updata for new prototypes
</commit_message>
<xml_diff>
--- a/IO_Dev/RunControl_Dev.xlsx
+++ b/IO_Dev/RunControl_Dev.xlsx
@@ -1465,7 +1465,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2197,7 +2197,7 @@
         <v>175</v>
       </c>
       <c r="C9" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
         <v>222</v>
@@ -2230,7 +2230,7 @@
         <v>212</v>
       </c>
       <c r="N9" s="27">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
       <c r="O9" s="19" t="b">
         <v>0</v>
@@ -2382,7 +2382,7 @@
         <v>212</v>
       </c>
       <c r="N10" s="27">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
       <c r="O10" s="19" t="b">
         <v>0</v>
@@ -2534,7 +2534,7 @@
         <v>212</v>
       </c>
       <c r="N11" s="27">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="O11" s="19" t="b">
         <v>0</v>

</xml_diff>